<commit_message>
added data for magnolia 2-319
</commit_message>
<xml_diff>
--- a/measured-trees.xlsx
+++ b/measured-trees.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\github\database\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="13290" windowHeight="14040" tabRatio="347"/>
   </bookViews>
@@ -18,7 +13,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">primary!$A$3:$P$104</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
@@ -29,7 +24,7 @@
     <author>Steven J Baskauf</author>
   </authors>
   <commentList>
-    <comment ref="I4" authorId="0" shapeId="0">
+    <comment ref="I4" authorId="0">
       <text>
         <r>
           <rPr>
@@ -53,7 +48,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E11" authorId="1" shapeId="0">
+    <comment ref="E11" authorId="1">
       <text>
         <r>
           <rPr>
@@ -77,7 +72,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H11" authorId="1" shapeId="0">
+    <comment ref="H11" authorId="1">
       <text>
         <r>
           <rPr>
@@ -101,7 +96,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I17" authorId="0" shapeId="0">
+    <comment ref="I17" authorId="0">
       <text>
         <r>
           <rPr>
@@ -125,7 +120,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H21" authorId="0" shapeId="0">
+    <comment ref="H21" authorId="0">
       <text>
         <r>
           <rPr>
@@ -149,7 +144,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E22" authorId="0" shapeId="0">
+    <comment ref="E22" authorId="0">
       <text>
         <r>
           <rPr>
@@ -173,7 +168,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H22" authorId="1" shapeId="0">
+    <comment ref="H22" authorId="1">
       <text>
         <r>
           <rPr>
@@ -197,7 +192,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I22" authorId="0" shapeId="0">
+    <comment ref="I22" authorId="0">
       <text>
         <r>
           <rPr>
@@ -221,7 +216,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K22" authorId="0" shapeId="0">
+    <comment ref="K22" authorId="0">
       <text>
         <r>
           <rPr>
@@ -245,7 +240,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A23" authorId="0" shapeId="0">
+    <comment ref="A23" authorId="0">
       <text>
         <r>
           <rPr>
@@ -269,7 +264,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I25" authorId="0" shapeId="0">
+    <comment ref="I25" authorId="0">
       <text>
         <r>
           <rPr>
@@ -293,7 +288,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I27" authorId="0" shapeId="0">
+    <comment ref="I27" authorId="0">
       <text>
         <r>
           <rPr>
@@ -317,7 +312,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E34" authorId="1" shapeId="0">
+    <comment ref="E34" authorId="1">
       <text>
         <r>
           <rPr>
@@ -341,7 +336,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H34" authorId="1" shapeId="0">
+    <comment ref="H34" authorId="1">
       <text>
         <r>
           <rPr>
@@ -365,7 +360,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I37" authorId="0" shapeId="0">
+    <comment ref="I38" authorId="0">
       <text>
         <r>
           <rPr>
@@ -389,7 +384,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H38" authorId="1" shapeId="0">
+    <comment ref="H39" authorId="1">
       <text>
         <r>
           <rPr>
@@ -413,7 +408,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K38" authorId="1" shapeId="0">
+    <comment ref="K39" authorId="1">
       <text>
         <r>
           <rPr>
@@ -437,7 +432,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I39" authorId="0" shapeId="0">
+    <comment ref="I40" authorId="0">
       <text>
         <r>
           <rPr>
@@ -461,7 +456,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I41" authorId="0" shapeId="0">
+    <comment ref="I42" authorId="0">
       <text>
         <r>
           <rPr>
@@ -485,7 +480,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E43" authorId="1" shapeId="0">
+    <comment ref="E44" authorId="1">
       <text>
         <r>
           <rPr>
@@ -509,7 +504,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H43" authorId="1" shapeId="0">
+    <comment ref="H44" authorId="1">
       <text>
         <r>
           <rPr>
@@ -533,7 +528,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B44" authorId="1" shapeId="0">
+    <comment ref="B45" authorId="1">
       <text>
         <r>
           <rPr>
@@ -557,7 +552,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H46" authorId="1" shapeId="0">
+    <comment ref="H47" authorId="1">
       <text>
         <r>
           <rPr>
@@ -581,7 +576,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I46" authorId="0" shapeId="0">
+    <comment ref="I47" authorId="0">
       <text>
         <r>
           <rPr>
@@ -605,7 +600,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K46" authorId="0" shapeId="0">
+    <comment ref="K47" authorId="0">
       <text>
         <r>
           <rPr>
@@ -629,7 +624,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E48" authorId="1" shapeId="0">
+    <comment ref="E49" authorId="1">
       <text>
         <r>
           <rPr>
@@ -653,7 +648,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H48" authorId="1" shapeId="0">
+    <comment ref="H49" authorId="1">
       <text>
         <r>
           <rPr>
@@ -677,7 +672,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H51" authorId="0" shapeId="0">
+    <comment ref="H52" authorId="0">
       <text>
         <r>
           <rPr>
@@ -701,7 +696,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H56" authorId="0" shapeId="0">
+    <comment ref="H57" authorId="0">
       <text>
         <r>
           <rPr>
@@ -725,7 +720,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E57" authorId="0" shapeId="0">
+    <comment ref="E58" authorId="0">
       <text>
         <r>
           <rPr>
@@ -749,7 +744,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="N57" authorId="1" shapeId="0">
+    <comment ref="N58" authorId="1">
       <text>
         <r>
           <rPr>
@@ -773,7 +768,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E58" authorId="1" shapeId="0">
+    <comment ref="E59" authorId="1">
       <text>
         <r>
           <rPr>
@@ -797,7 +792,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H59" authorId="0" shapeId="0">
+    <comment ref="H60" authorId="0">
       <text>
         <r>
           <rPr>
@@ -821,7 +816,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E60" authorId="1" shapeId="0">
+    <comment ref="E61" authorId="1">
       <text>
         <r>
           <rPr>
@@ -845,7 +840,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H60" authorId="1" shapeId="0">
+    <comment ref="H61" authorId="1">
       <text>
         <r>
           <rPr>
@@ -869,7 +864,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E62" authorId="1" shapeId="0">
+    <comment ref="E63" authorId="1">
       <text>
         <r>
           <rPr>
@@ -893,7 +888,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H62" authorId="1" shapeId="0">
+    <comment ref="H63" authorId="1">
       <text>
         <r>
           <rPr>
@@ -917,7 +912,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K62" authorId="1" shapeId="0">
+    <comment ref="K63" authorId="1">
       <text>
         <r>
           <rPr>
@@ -941,7 +936,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="N62" authorId="1" shapeId="0">
+    <comment ref="N63" authorId="1">
       <text>
         <r>
           <rPr>
@@ -965,7 +960,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A72" authorId="0" shapeId="0">
+    <comment ref="A72" authorId="0">
       <text>
         <r>
           <rPr>
@@ -989,7 +984,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A82" authorId="0" shapeId="0">
+    <comment ref="A82" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1013,7 +1008,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E105" authorId="1" shapeId="0">
+    <comment ref="E105" authorId="1">
       <text>
         <r>
           <rPr>
@@ -1037,7 +1032,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B107" authorId="0" shapeId="0">
+    <comment ref="B107" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1061,7 +1056,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E108" authorId="0" shapeId="0">
+    <comment ref="E108" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1090,7 +1085,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="783" uniqueCount="427">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="785" uniqueCount="427">
   <si>
     <t>ID</t>
   </si>
@@ -2961,7 +2956,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2972,11 +2967,11 @@
   <dimension ref="A1:Q684"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <pane xSplit="3330" ySplit="600" topLeftCell="C68" activePane="bottomRight"/>
+      <pane xSplit="3330" ySplit="600" topLeftCell="G32" activePane="bottomLeft"/>
       <selection activeCell="A22" sqref="A22"/>
       <selection pane="topRight" activeCell="K3" sqref="K3"/>
-      <selection pane="bottomLeft" activeCell="A72" sqref="A72:XFD72"/>
-      <selection pane="bottomRight" activeCell="P91" sqref="P91"/>
+      <selection pane="bottomLeft" activeCell="A37" sqref="A37:XFD37"/>
+      <selection pane="bottomRight" activeCell="H68" sqref="H68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4871,1635 +4866,1644 @@
       </c>
       <c r="Q36" s="6"/>
     </row>
-    <row r="37" spans="1:17" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="2" t="s">
+    <row r="37" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A37" s="131" t="s">
+        <v>56</v>
+      </c>
+      <c r="B37" s="131" t="s">
+        <v>55</v>
+      </c>
+      <c r="C37" s="132">
+        <v>36.146718</v>
+      </c>
+      <c r="D37" s="132">
+        <v>-86.802537000000001</v>
+      </c>
+      <c r="E37" s="26" t="s">
+        <v>77</v>
+      </c>
+      <c r="F37" s="26">
+        <f>E37/2.54</f>
+        <v>46.45669291338583</v>
+      </c>
+      <c r="G37" s="24" t="s">
+        <v>104</v>
+      </c>
+      <c r="H37" s="13">
+        <v>20</v>
+      </c>
+      <c r="I37" s="21">
+        <f>H37*3.281</f>
+        <v>65.62</v>
+      </c>
+      <c r="J37" s="134" t="s">
+        <v>414</v>
+      </c>
+      <c r="K37" s="29">
+        <v>16.5</v>
+      </c>
+      <c r="L37" s="30">
+        <f>K37*3.281</f>
+        <v>54.136500000000005</v>
+      </c>
+      <c r="M37" s="134" t="s">
+        <v>414</v>
+      </c>
+      <c r="N37" s="15">
+        <f>IF(K37=0,0,E37/2.54*3.14159+H37*3.281+K37*3.281/4)</f>
+        <v>225.10200688976377</v>
+      </c>
+      <c r="O37" s="131" t="s">
+        <v>89</v>
+      </c>
+      <c r="P37" s="129" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="38" spans="1:17" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="B37" s="7" t="s">
+      <c r="B38" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="C37">
+      <c r="C38">
         <v>36.145836000000003</v>
       </c>
-      <c r="D37">
+      <c r="D38">
         <v>-86.802235999999994</v>
       </c>
-      <c r="E37" s="26" t="s">
+      <c r="E38" s="26" t="s">
         <v>118</v>
       </c>
-      <c r="F37" s="26">
+      <c r="F38" s="26">
         <f t="shared" si="5"/>
         <v>42.913385826771652</v>
       </c>
-      <c r="G37" s="24" t="s">
+      <c r="G38" s="24" t="s">
         <v>104</v>
       </c>
-      <c r="H37" s="13">
-        <f>I37/3.281</f>
+      <c r="H38" s="13">
+        <f>I38/3.281</f>
         <v>22.005486132276744</v>
       </c>
-      <c r="I37" s="23">
+      <c r="I38" s="23">
         <v>72.2</v>
       </c>
-      <c r="J37" s="2" t="s">
+      <c r="J38" s="2" t="s">
         <v>401</v>
       </c>
-      <c r="K37" s="36">
+      <c r="K38" s="36">
         <v>19</v>
       </c>
-      <c r="L37" s="37">
+      <c r="L38" s="37">
         <f t="shared" si="6"/>
         <v>62.339000000000006</v>
       </c>
-      <c r="M37" s="35" t="s">
+      <c r="M38" s="35" t="s">
         <v>401</v>
       </c>
-      <c r="N37" s="15">
+      <c r="N38" s="15">
         <f t="shared" si="7"/>
         <v>222.60101377952756</v>
       </c>
-      <c r="O37" s="2" t="s">
+      <c r="O38" s="2" t="s">
         <v>331</v>
       </c>
-      <c r="P37" t="s">
+      <c r="P38" t="s">
         <v>366</v>
       </c>
-      <c r="Q37" s="6"/>
-    </row>
-    <row r="38" spans="1:17" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="2" t="s">
+      <c r="Q38" s="6"/>
+    </row>
+    <row r="39" spans="1:17" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="B38" s="2" t="s">
+      <c r="B39" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="C38" s="3">
+      <c r="C39" s="3">
         <v>36.147970000000001</v>
       </c>
-      <c r="D38" s="3">
+      <c r="D39" s="3">
         <v>-86.802019000000001</v>
       </c>
-      <c r="E38" s="26" t="s">
+      <c r="E39" s="26" t="s">
         <v>84</v>
       </c>
-      <c r="F38" s="26">
+      <c r="F39" s="26">
         <f t="shared" si="5"/>
         <v>40.944881889763778</v>
       </c>
-      <c r="G38" s="24" t="s">
+      <c r="G39" s="24" t="s">
         <v>103</v>
       </c>
-      <c r="H38" s="13">
+      <c r="H39" s="13">
         <v>23.67</v>
       </c>
-      <c r="I38" s="21">
-        <f>H38*3.281</f>
+      <c r="I39" s="21">
+        <f>H39*3.281</f>
         <v>77.661270000000002</v>
       </c>
-      <c r="J38" s="7" t="s">
+      <c r="J39" s="7" t="s">
         <v>377</v>
       </c>
-      <c r="K38" s="29">
+      <c r="K39" s="29">
         <v>17.07</v>
       </c>
-      <c r="L38" s="30">
+      <c r="L39" s="30">
         <f t="shared" si="6"/>
         <v>56.006670000000007</v>
       </c>
-      <c r="M38" s="31" t="s">
+      <c r="M39" s="31" t="s">
         <v>377</v>
       </c>
-      <c r="N38" s="33">
+      <c r="N39" s="33">
         <f t="shared" si="7"/>
         <v>220.29496899606298</v>
       </c>
-      <c r="O38" s="2" t="s">
+      <c r="O39" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="P38" s="2" t="s">
+      <c r="P39" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="Q38" s="6"/>
-    </row>
-    <row r="39" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A39" s="7" t="s">
+      <c r="Q39" s="6"/>
+    </row>
+    <row r="40" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A40" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="B39" s="10" t="s">
+      <c r="B40" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="C39" s="8">
+      <c r="C40" s="8">
         <v>36.146864000000001</v>
       </c>
-      <c r="D39" s="8">
+      <c r="D40" s="8">
         <v>-86.801839000000001</v>
       </c>
-      <c r="E39" s="26" t="s">
+      <c r="E40" s="26" t="s">
         <v>82</v>
       </c>
-      <c r="F39" s="26">
+      <c r="F40" s="26">
         <f t="shared" si="5"/>
         <v>32.677165354330711</v>
       </c>
-      <c r="G39" s="24" t="s">
+      <c r="G40" s="24" t="s">
         <v>103</v>
       </c>
-      <c r="H39" s="13">
-        <f>I39/3.281</f>
+      <c r="H40" s="13">
+        <f>I40/3.281</f>
         <v>28.649801889667781</v>
       </c>
-      <c r="I39" s="23">
+      <c r="I40" s="23">
         <v>94</v>
       </c>
-      <c r="J39" s="7" t="s">
+      <c r="J40" s="7" t="s">
         <v>318</v>
       </c>
-      <c r="K39" s="29">
+      <c r="K40" s="29">
         <v>20.5</v>
       </c>
-      <c r="L39" s="30">
+      <c r="L40" s="30">
         <f t="shared" si="6"/>
         <v>67.260500000000008</v>
       </c>
-      <c r="M39" s="27" t="s">
+      <c r="M40" s="27" t="s">
         <v>318</v>
       </c>
-      <c r="N39" s="15">
+      <c r="N40" s="15">
         <f t="shared" si="7"/>
         <v>213.47338090551179</v>
       </c>
-      <c r="O39" s="7" t="s">
+      <c r="O40" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="P39" s="1" t="s">
+      <c r="P40" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="40" spans="1:17" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="61" t="s">
+    <row r="41" spans="1:17" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="61" t="s">
         <v>100</v>
       </c>
-      <c r="B40" s="134" t="s">
+      <c r="B41" s="134" t="s">
         <v>55</v>
       </c>
-      <c r="C40" s="132">
+      <c r="C41" s="132">
         <v>36.145913999999998</v>
       </c>
-      <c r="D40" s="132">
+      <c r="D41" s="132">
         <v>-86.801046999999997</v>
       </c>
-      <c r="E40" s="63" t="s">
+      <c r="E41" s="63" t="s">
         <v>86</v>
       </c>
-      <c r="F40" s="66">
+      <c r="F41" s="66">
         <f t="shared" si="5"/>
         <v>43.30708661417323</v>
       </c>
-      <c r="G40" s="145" t="s">
+      <c r="G41" s="145" t="s">
         <v>104</v>
       </c>
-      <c r="H40" s="62">
+      <c r="H41" s="62">
         <v>18.5</v>
       </c>
-      <c r="I40" s="65">
-        <f>H40*3.281</f>
+      <c r="I41" s="65">
+        <f>H41*3.281</f>
         <v>60.698500000000003</v>
       </c>
-      <c r="J40" s="61" t="s">
+      <c r="J41" s="61" t="s">
         <v>414</v>
       </c>
-      <c r="K40" s="159">
+      <c r="K41" s="159">
         <v>17.75</v>
       </c>
-      <c r="L40" s="67">
+      <c r="L41" s="67">
         <f t="shared" si="6"/>
         <v>58.237750000000005</v>
       </c>
-      <c r="M40" s="134" t="s">
+      <c r="M41" s="134" t="s">
         <v>414</v>
       </c>
-      <c r="N40" s="64">
+      <c r="N41" s="64">
         <f t="shared" si="7"/>
         <v>211.31104773622047</v>
       </c>
-      <c r="O40" s="134" t="s">
+      <c r="O41" s="134" t="s">
         <v>330</v>
       </c>
-      <c r="P40" s="129" t="s">
+      <c r="P41" s="129" t="s">
         <v>365</v>
       </c>
-      <c r="Q40" s="6"/>
-    </row>
-    <row r="41" spans="1:17" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="7" t="s">
+      <c r="Q41" s="6"/>
+    </row>
+    <row r="42" spans="1:17" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="7" t="s">
         <v>135</v>
       </c>
-      <c r="B41" s="10" t="s">
+      <c r="B42" s="10" t="s">
         <v>136</v>
       </c>
-      <c r="C41">
+      <c r="C42">
         <v>36.146563999999998</v>
       </c>
-      <c r="D41">
+      <c r="D42">
         <v>-86.801297000000005</v>
       </c>
-      <c r="E41" s="26" t="s">
+      <c r="E42" s="26" t="s">
         <v>75</v>
       </c>
-      <c r="F41" s="26">
+      <c r="F42" s="26">
         <f t="shared" si="5"/>
         <v>43.7007874015748</v>
       </c>
-      <c r="G41" s="24" t="s">
+      <c r="G42" s="24" t="s">
         <v>128</v>
       </c>
-      <c r="H41" s="13">
-        <f>I41/3.281</f>
+      <c r="H42" s="13">
+        <f>I42/3.281</f>
         <v>18.40902163974398</v>
       </c>
-      <c r="I41" s="23">
+      <c r="I42" s="23">
         <v>60.4</v>
       </c>
-      <c r="J41" s="2" t="s">
+      <c r="J42" s="2" t="s">
         <v>401</v>
       </c>
-      <c r="K41" s="36">
+      <c r="K42" s="36">
         <v>16</v>
       </c>
-      <c r="L41" s="37">
+      <c r="L42" s="37">
         <f t="shared" si="6"/>
         <v>52.496000000000002</v>
       </c>
-      <c r="M41" s="35" t="s">
+      <c r="M42" s="35" t="s">
         <v>401</v>
       </c>
-      <c r="N41" s="15">
+      <c r="N42" s="15">
         <f t="shared" si="7"/>
         <v>210.81395669291337</v>
       </c>
-      <c r="O41" s="7" t="s">
+      <c r="O42" s="7" t="s">
         <v>137</v>
       </c>
-      <c r="P41" t="s">
+      <c r="P42" t="s">
         <v>364</v>
       </c>
-      <c r="Q41" s="6"/>
-    </row>
-    <row r="42" spans="1:17" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="7" t="s">
+      <c r="Q42" s="6"/>
+    </row>
+    <row r="43" spans="1:17" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="7" t="s">
         <v>141</v>
       </c>
-      <c r="B42" s="134" t="s">
+      <c r="B43" s="134" t="s">
         <v>55</v>
       </c>
-      <c r="C42" s="129">
+      <c r="C43" s="129">
         <v>36.146968000000001</v>
       </c>
-      <c r="D42" s="129">
+      <c r="D43" s="129">
         <v>-86.801186000000001</v>
       </c>
-      <c r="E42" s="26" t="s">
+      <c r="E43" s="26" t="s">
         <v>118</v>
       </c>
-      <c r="F42" s="26">
+      <c r="F43" s="26">
         <f t="shared" si="5"/>
         <v>42.913385826771652</v>
       </c>
-      <c r="G42" s="24" t="s">
+      <c r="G43" s="24" t="s">
         <v>128</v>
       </c>
-      <c r="H42" s="13">
+      <c r="H43" s="13">
         <v>18.5</v>
       </c>
-      <c r="I42" s="21">
-        <f>H42*3.281</f>
+      <c r="I43" s="21">
+        <f>H43*3.281</f>
         <v>60.698500000000003</v>
       </c>
-      <c r="J42" s="134" t="s">
+      <c r="J43" s="134" t="s">
         <v>414</v>
       </c>
-      <c r="K42" s="29">
+      <c r="K43" s="29">
         <v>16</v>
       </c>
-      <c r="L42" s="30">
+      <c r="L43" s="30">
         <f t="shared" si="6"/>
         <v>52.496000000000002</v>
       </c>
-      <c r="M42" s="150" t="s">
+      <c r="M43" s="150" t="s">
         <v>414</v>
       </c>
-      <c r="N42" s="15">
+      <c r="N43" s="15">
         <f t="shared" si="7"/>
         <v>208.63876377952755</v>
       </c>
-      <c r="O42" s="7" t="s">
+      <c r="O43" s="7" t="s">
         <v>142</v>
       </c>
-      <c r="P42" t="s">
+      <c r="P43" t="s">
         <v>367</v>
       </c>
-      <c r="Q42" s="6"/>
-    </row>
-    <row r="43" spans="1:17" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="7" t="s">
+      <c r="Q43" s="6"/>
+    </row>
+    <row r="44" spans="1:17" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="7" t="s">
         <v>383</v>
       </c>
-      <c r="B43" s="130" t="s">
+      <c r="B44" s="130" t="s">
         <v>55</v>
       </c>
-      <c r="C43" s="129">
+      <c r="C44" s="129">
         <v>36.148797999999999</v>
       </c>
-      <c r="D43" s="129">
+      <c r="D44" s="129">
         <v>-86.801866000000004</v>
       </c>
-      <c r="E43" s="26">
+      <c r="E44" s="26">
         <v>106</v>
       </c>
-      <c r="F43" s="26">
+      <c r="F44" s="26">
         <f t="shared" si="5"/>
         <v>41.732283464566926</v>
       </c>
-      <c r="G43" s="150" t="s">
+      <c r="G44" s="150" t="s">
         <v>414</v>
       </c>
-      <c r="H43" s="13">
+      <c r="H44" s="13">
         <v>19</v>
       </c>
-      <c r="I43" s="21">
-        <f>H43*3.281</f>
+      <c r="I44" s="21">
+        <f>H44*3.281</f>
         <v>62.339000000000006</v>
       </c>
-      <c r="J43" s="134" t="s">
+      <c r="J44" s="134" t="s">
         <v>414</v>
       </c>
-      <c r="K43" s="158">
+      <c r="K44" s="158">
         <v>17.25</v>
       </c>
-      <c r="L43" s="30">
+      <c r="L44" s="30">
         <f t="shared" si="6"/>
         <v>56.597250000000003</v>
       </c>
-      <c r="M43" s="150" t="s">
+      <c r="M44" s="150" t="s">
         <v>414</v>
       </c>
-      <c r="N43" s="15">
+      <c r="N44" s="15">
         <f t="shared" si="7"/>
         <v>207.59403690944882</v>
       </c>
-      <c r="O43" s="130" t="s">
+      <c r="O44" s="130" t="s">
         <v>402</v>
       </c>
-      <c r="P43" s="1" t="s">
+      <c r="P44" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="Q43" s="6"/>
-    </row>
-    <row r="44" spans="1:17" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="7" t="s">
+      <c r="Q44" s="6"/>
+    </row>
+    <row r="45" spans="1:17" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="7" t="s">
         <v>192</v>
       </c>
-      <c r="B44" s="131" t="s">
+      <c r="B45" s="131" t="s">
         <v>66</v>
       </c>
-      <c r="C44" s="3">
+      <c r="C45" s="3">
         <v>36.148634000000001</v>
       </c>
-      <c r="D44" s="3">
+      <c r="D45" s="3">
         <v>-86.801985999999999</v>
       </c>
-      <c r="E44" s="26" t="s">
+      <c r="E45" s="26" t="s">
         <v>193</v>
       </c>
-      <c r="F44" s="26">
+      <c r="F45" s="26">
         <f t="shared" si="5"/>
         <v>39.763779527559052</v>
       </c>
-      <c r="G44" s="24" t="s">
+      <c r="G45" s="24" t="s">
         <v>196</v>
       </c>
-      <c r="H44" s="13">
+      <c r="H45" s="13">
         <v>19.5</v>
       </c>
-      <c r="I44" s="21">
-        <f>H44*3.281</f>
+      <c r="I45" s="21">
+        <f>H45*3.281</f>
         <v>63.979500000000002</v>
       </c>
-      <c r="J44" s="131" t="s">
+      <c r="J45" s="131" t="s">
         <v>340</v>
       </c>
-      <c r="K44" s="159">
+      <c r="K45" s="159">
         <v>18</v>
       </c>
-      <c r="L44" s="161">
+      <c r="L45" s="161">
         <f t="shared" si="6"/>
         <v>59.058</v>
       </c>
-      <c r="M44" s="152" t="s">
+      <c r="M45" s="152" t="s">
         <v>340</v>
       </c>
-      <c r="N44" s="15">
+      <c r="N45" s="15">
         <f t="shared" si="7"/>
         <v>203.66549212598426</v>
       </c>
-      <c r="O44" s="7" t="s">
+      <c r="O45" s="7" t="s">
         <v>194</v>
       </c>
-      <c r="P44" s="129" t="s">
+      <c r="P45" s="129" t="s">
         <v>359</v>
       </c>
-      <c r="Q44" s="6"/>
-    </row>
-    <row r="45" spans="1:17" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="134" t="s">
+      <c r="Q45" s="6"/>
+    </row>
+    <row r="46" spans="1:17" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="134" t="s">
         <v>96</v>
       </c>
-      <c r="B45" s="137" t="s">
+      <c r="B46" s="137" t="s">
         <v>98</v>
       </c>
-      <c r="C45" s="132">
+      <c r="C46" s="132">
         <v>36.148558999999999</v>
       </c>
-      <c r="D45" s="132">
+      <c r="D46" s="132">
         <v>-86.803090999999995</v>
       </c>
-      <c r="E45" s="26" t="s">
+      <c r="E46" s="26" t="s">
         <v>85</v>
       </c>
-      <c r="F45" s="26">
+      <c r="F46" s="26">
         <f t="shared" si="5"/>
         <v>39.370078740157481</v>
       </c>
-      <c r="G45" s="145" t="s">
+      <c r="G46" s="145" t="s">
         <v>104</v>
       </c>
-      <c r="H45" s="13">
+      <c r="H46" s="13">
         <v>18</v>
       </c>
-      <c r="I45" s="21">
-        <f>H45*3.281</f>
+      <c r="I46" s="21">
+        <f>H46*3.281</f>
         <v>59.058</v>
       </c>
-      <c r="J45" s="157" t="s">
+      <c r="J46" s="157" t="s">
         <v>340</v>
       </c>
-      <c r="K45" s="29">
+      <c r="K46" s="29">
         <v>23.5</v>
       </c>
-      <c r="L45" s="30">
+      <c r="L46" s="30">
         <f t="shared" si="6"/>
         <v>77.103499999999997</v>
       </c>
-      <c r="M45" s="147" t="s">
+      <c r="M46" s="147" t="s">
         <v>340</v>
       </c>
-      <c r="N45" s="15">
+      <c r="N46" s="15">
         <f t="shared" si="7"/>
         <v>202.01852066929132</v>
       </c>
-      <c r="O45" s="134" t="s">
+      <c r="O46" s="134" t="s">
         <v>99</v>
       </c>
-      <c r="P45" s="1" t="s">
+      <c r="P46" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="Q45" s="6"/>
-    </row>
-    <row r="46" spans="1:17" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="134" t="s">
+      <c r="Q46" s="6"/>
+    </row>
+    <row r="47" spans="1:17" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="134" t="s">
         <v>92</v>
       </c>
-      <c r="B46" s="7" t="s">
+      <c r="B47" s="7" t="s">
         <v>93</v>
       </c>
-      <c r="C46" s="132">
+      <c r="C47" s="132">
         <v>36.148681000000003</v>
       </c>
-      <c r="D46" s="132">
+      <c r="D47" s="132">
         <v>-86.802809999999994</v>
       </c>
-      <c r="E46" s="26" t="s">
+      <c r="E47" s="26" t="s">
         <v>94</v>
       </c>
-      <c r="F46" s="26">
+      <c r="F47" s="26">
         <f t="shared" si="5"/>
         <v>37.401574803149607</v>
       </c>
-      <c r="G46" s="24" t="s">
+      <c r="G47" s="24" t="s">
         <v>104</v>
       </c>
-      <c r="H46" s="13">
-        <f>I46/3.281</f>
+      <c r="H47" s="13">
+        <f>I47/3.281</f>
         <v>19.597683633038706</v>
       </c>
-      <c r="I46" s="21">
+      <c r="I47" s="21">
         <v>64.3</v>
       </c>
-      <c r="J46" s="7" t="s">
+      <c r="J47" s="7" t="s">
         <v>377</v>
       </c>
-      <c r="K46" s="148">
+      <c r="K47" s="148">
         <v>23</v>
       </c>
-      <c r="L46" s="149">
+      <c r="L47" s="149">
         <f t="shared" si="6"/>
         <v>75.463000000000008</v>
       </c>
-      <c r="M46" s="150" t="s">
+      <c r="M47" s="150" t="s">
         <v>377</v>
       </c>
-      <c r="N46" s="15">
+      <c r="N47" s="15">
         <f t="shared" si="7"/>
         <v>200.66616338582676</v>
       </c>
-      <c r="O46" s="134" t="s">
+      <c r="O47" s="134" t="s">
         <v>95</v>
       </c>
-      <c r="P46" s="134" t="s">
+      <c r="P47" s="134" t="s">
         <v>34</v>
       </c>
-      <c r="Q46" s="6"/>
-    </row>
-    <row r="47" spans="1:17" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="7" t="s">
+      <c r="Q47" s="6"/>
+    </row>
+    <row r="48" spans="1:17" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="7" t="s">
         <v>416</v>
       </c>
-      <c r="B47" s="130" t="s">
+      <c r="B48" s="130" t="s">
         <v>55</v>
       </c>
-      <c r="C47">
+      <c r="C48">
         <v>36.148344000000002</v>
       </c>
-      <c r="D47">
+      <c r="D48">
         <v>-86.802238000000003</v>
       </c>
-      <c r="E47" s="26">
+      <c r="E48" s="26">
         <v>107</v>
       </c>
-      <c r="F47" s="26">
+      <c r="F48" s="26">
         <f t="shared" si="5"/>
         <v>42.125984251968504</v>
       </c>
-      <c r="G47" s="150" t="s">
+      <c r="G48" s="150" t="s">
         <v>414</v>
       </c>
-      <c r="H47" s="140">
+      <c r="H48" s="140">
         <v>15</v>
       </c>
-      <c r="I47" s="21">
-        <f t="shared" ref="I47:I78" si="8">H47*3.281</f>
+      <c r="I48" s="21">
+        <f t="shared" ref="I48:I78" si="8">H48*3.281</f>
         <v>49.215000000000003</v>
       </c>
-      <c r="J47" s="134" t="s">
+      <c r="J48" s="134" t="s">
         <v>414</v>
       </c>
-      <c r="K47" s="148">
+      <c r="K48" s="148">
         <v>15.25</v>
       </c>
-      <c r="L47" s="149">
+      <c r="L48" s="149">
         <f t="shared" si="6"/>
         <v>50.035250000000005</v>
       </c>
-      <c r="M47" s="150" t="s">
+      <c r="M48" s="150" t="s">
         <v>414</v>
       </c>
-      <c r="N47" s="15">
+      <c r="N48" s="15">
         <f t="shared" si="7"/>
         <v>194.06638336614174</v>
       </c>
-      <c r="O47" s="130" t="s">
+      <c r="O48" s="130" t="s">
         <v>417</v>
       </c>
-      <c r="P47" s="1" t="s">
+      <c r="P48" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="Q47" s="6"/>
-    </row>
-    <row r="48" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A48" s="131" t="s">
+      <c r="Q48" s="6"/>
+    </row>
+    <row r="49" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A49" s="131" t="s">
         <v>381</v>
       </c>
-      <c r="B48" s="130" t="s">
+      <c r="B49" s="130" t="s">
         <v>66</v>
       </c>
-      <c r="C48">
+      <c r="C49">
         <v>36.148788000000003</v>
       </c>
-      <c r="D48">
+      <c r="D49">
         <v>-86.803242999999995</v>
       </c>
-      <c r="E48" s="26">
+      <c r="E49" s="26">
         <v>95.5</v>
       </c>
-      <c r="F48" s="26">
+      <c r="F49" s="26">
         <f t="shared" si="5"/>
         <v>37.598425196850393</v>
       </c>
-      <c r="G48" s="150" t="s">
+      <c r="G49" s="150" t="s">
         <v>377</v>
       </c>
-      <c r="H48" s="13">
+      <c r="H49" s="13">
         <v>16.78</v>
       </c>
-      <c r="I48" s="21">
+      <c r="I49" s="21">
         <f t="shared" si="8"/>
         <v>55.055180000000007</v>
       </c>
-      <c r="J48" s="134" t="s">
+      <c r="J49" s="134" t="s">
         <v>377</v>
       </c>
-      <c r="K48" s="159">
+      <c r="K49" s="159">
         <v>21.25</v>
       </c>
-      <c r="L48" s="161">
+      <c r="L49" s="161">
         <f t="shared" si="6"/>
         <v>69.721249999999998</v>
       </c>
-      <c r="M48" s="134" t="s">
+      <c r="M49" s="134" t="s">
         <v>377</v>
       </c>
-      <c r="N48" s="15">
+      <c r="N49" s="15">
         <f t="shared" si="7"/>
         <v>190.60432911417325</v>
       </c>
-      <c r="O48" s="1" t="s">
+      <c r="O49" s="1" t="s">
         <v>393</v>
       </c>
-      <c r="P48" s="130" t="s">
+      <c r="P49" s="130" t="s">
         <v>399</v>
       </c>
     </row>
-    <row r="49" spans="1:17" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="130" t="s">
+    <row r="50" spans="1:17" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="130" t="s">
         <v>182</v>
       </c>
-      <c r="B49" s="134" t="s">
+      <c r="B50" s="134" t="s">
         <v>55</v>
       </c>
-      <c r="C49">
+      <c r="C50">
         <v>36.142912000000003</v>
       </c>
-      <c r="D49">
+      <c r="D50">
         <v>-86.798676</v>
       </c>
-      <c r="E49" s="26" t="s">
+      <c r="E50" s="26" t="s">
         <v>181</v>
       </c>
-      <c r="F49" s="26">
+      <c r="F50" s="26">
         <f t="shared" si="5"/>
         <v>37.204724409448815</v>
       </c>
-      <c r="G49" s="24" t="s">
+      <c r="G50" s="24" t="s">
         <v>128</v>
       </c>
-      <c r="H49" s="140">
+      <c r="H50" s="140">
         <v>18.100000000000001</v>
       </c>
-      <c r="I49" s="21">
+      <c r="I50" s="21">
         <f t="shared" si="8"/>
         <v>59.386100000000006</v>
       </c>
-      <c r="J49" s="150" t="s">
+      <c r="J50" s="150" t="s">
         <v>403</v>
       </c>
-      <c r="K49" s="148">
+      <c r="K50" s="148">
         <v>13.5</v>
       </c>
-      <c r="L49" s="149">
+      <c r="L50" s="149">
         <f t="shared" si="6"/>
         <v>44.293500000000002</v>
       </c>
-      <c r="M49" s="147" t="s">
+      <c r="M50" s="147" t="s">
         <v>403</v>
       </c>
-      <c r="N49" s="15">
+      <c r="N50" s="15">
         <f t="shared" si="7"/>
         <v>187.34146515748031</v>
       </c>
-      <c r="O49" s="130" t="s">
+      <c r="O50" s="130" t="s">
         <v>183</v>
       </c>
-      <c r="P49" t="s">
+      <c r="P50" t="s">
         <v>409</v>
       </c>
-      <c r="Q49" s="6"/>
-    </row>
-    <row r="50" spans="1:17" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="130" t="s">
+      <c r="Q50" s="6"/>
+    </row>
+    <row r="51" spans="1:17" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="130" t="s">
         <v>143</v>
       </c>
-      <c r="B50" s="134" t="s">
+      <c r="B51" s="134" t="s">
         <v>55</v>
       </c>
-      <c r="C50" s="129">
+      <c r="C51" s="129">
         <v>36.146942000000003</v>
       </c>
-      <c r="D50" s="129">
+      <c r="D51" s="129">
         <v>-86.801242999999999</v>
       </c>
-      <c r="E50" s="26" t="s">
+      <c r="E51" s="26" t="s">
         <v>144</v>
       </c>
-      <c r="F50" s="26">
+      <c r="F51" s="26">
         <f t="shared" si="5"/>
         <v>33.464566929133859</v>
       </c>
-      <c r="G50" s="24" t="s">
+      <c r="G51" s="24" t="s">
         <v>128</v>
       </c>
-      <c r="H50" s="140">
+      <c r="H51" s="140">
         <v>19</v>
       </c>
-      <c r="I50" s="21">
+      <c r="I51" s="21">
         <f t="shared" si="8"/>
         <v>62.339000000000006</v>
       </c>
-      <c r="J50" s="150" t="s">
+      <c r="J51" s="150" t="s">
         <v>414</v>
       </c>
-      <c r="K50" s="159">
+      <c r="K51" s="159">
         <v>21.25</v>
       </c>
-      <c r="L50" s="161">
+      <c r="L51" s="161">
         <f t="shared" si="6"/>
         <v>69.721249999999998</v>
       </c>
-      <c r="M50" s="150" t="s">
+      <c r="M51" s="150" t="s">
         <v>414</v>
       </c>
-      <c r="N50" s="15">
+      <c r="N51" s="15">
         <f t="shared" si="7"/>
         <v>184.90126131889764</v>
       </c>
-      <c r="O50" s="7" t="s">
+      <c r="O51" s="7" t="s">
         <v>145</v>
       </c>
-      <c r="P50" t="s">
+      <c r="P51" t="s">
         <v>418</v>
       </c>
-      <c r="Q50" s="6"/>
-    </row>
-    <row r="51" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A51" s="40" t="s">
+      <c r="Q51" s="6"/>
+    </row>
+    <row r="52" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A52" s="40" t="s">
         <v>130</v>
       </c>
-      <c r="B51" s="137" t="s">
+      <c r="B52" s="137" t="s">
         <v>131</v>
       </c>
-      <c r="C51" s="38">
+      <c r="C52" s="38">
         <v>36.146026999999997</v>
       </c>
-      <c r="D51" s="38">
+      <c r="D52" s="38">
         <v>-86.802841999999998</v>
       </c>
-      <c r="E51" s="43" t="s">
+      <c r="E52" s="43" t="s">
         <v>133</v>
       </c>
-      <c r="F51" s="43">
+      <c r="F52" s="43">
         <f t="shared" si="5"/>
         <v>38.188976377952756</v>
       </c>
-      <c r="G51" s="145" t="s">
+      <c r="G52" s="145" t="s">
         <v>128</v>
       </c>
-      <c r="H51" s="156">
+      <c r="H52" s="156">
         <v>13.5</v>
       </c>
-      <c r="I51" s="42">
+      <c r="I52" s="42">
         <f t="shared" si="8"/>
         <v>44.293500000000002</v>
       </c>
-      <c r="J51" s="131" t="s">
+      <c r="J52" s="131" t="s">
         <v>401</v>
       </c>
-      <c r="K51" s="158">
+      <c r="K52" s="158">
         <v>22.5</v>
       </c>
-      <c r="L51" s="160">
+      <c r="L52" s="160">
         <f t="shared" si="6"/>
         <v>73.822500000000005</v>
       </c>
-      <c r="M51" s="157" t="s">
+      <c r="M52" s="157" t="s">
         <v>401</v>
       </c>
-      <c r="N51" s="41">
+      <c r="N52" s="41">
         <f t="shared" si="7"/>
         <v>182.72323129921259</v>
       </c>
-      <c r="O51" s="134" t="s">
+      <c r="O52" s="134" t="s">
         <v>134</v>
       </c>
-      <c r="P51" s="39" t="s">
+      <c r="P52" s="39" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="52" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A52" s="134" t="s">
+    <row r="53" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A53" s="134" t="s">
         <v>419</v>
       </c>
-      <c r="B52" s="1" t="s">
+      <c r="B53" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="C52">
+      <c r="C53">
         <v>36.148625000000003</v>
       </c>
-      <c r="D52">
+      <c r="D53">
         <v>-86.802114000000003</v>
       </c>
-      <c r="E52" s="26">
+      <c r="E53" s="26">
         <v>89</v>
       </c>
-      <c r="F52" s="26">
+      <c r="F53" s="26">
         <f t="shared" si="5"/>
         <v>35.039370078740156</v>
       </c>
-      <c r="G52" s="150" t="s">
+      <c r="G53" s="150" t="s">
         <v>414</v>
       </c>
-      <c r="H52" s="13">
+      <c r="H53" s="13">
         <v>18</v>
       </c>
-      <c r="I52" s="21">
+      <c r="I53" s="21">
         <f t="shared" si="8"/>
         <v>59.058</v>
       </c>
-      <c r="J52" s="7" t="s">
+      <c r="J53" s="7" t="s">
         <v>414</v>
       </c>
-      <c r="K52" s="29">
+      <c r="K53" s="29">
         <v>15</v>
       </c>
-      <c r="L52" s="30">
+      <c r="L53" s="30">
         <f t="shared" si="6"/>
         <v>49.215000000000003</v>
       </c>
-      <c r="M52" s="31" t="s">
+      <c r="M53" s="31" t="s">
         <v>414</v>
       </c>
-      <c r="N52" s="15">
+      <c r="N53" s="15">
         <f t="shared" si="7"/>
         <v>181.44108464566929</v>
       </c>
-      <c r="O52" s="1" t="s">
+      <c r="O53" s="1" t="s">
         <v>420</v>
       </c>
-      <c r="P52" s="1" t="s">
+      <c r="P53" s="1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="53" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A53" s="134" t="s">
+    <row r="54" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A54" s="134" t="s">
         <v>421</v>
       </c>
-      <c r="B53" s="130" t="s">
+      <c r="B54" s="130" t="s">
         <v>55</v>
       </c>
-      <c r="C53">
+      <c r="C54">
         <v>36.148536</v>
       </c>
-      <c r="D53">
+      <c r="D54">
         <v>-86.802197000000007</v>
       </c>
-      <c r="E53" s="26">
+      <c r="E54" s="26">
         <v>83</v>
       </c>
-      <c r="F53" s="26">
+      <c r="F54" s="26">
         <f t="shared" si="5"/>
         <v>32.677165354330711</v>
       </c>
-      <c r="G53" s="134" t="s">
+      <c r="G54" s="134" t="s">
         <v>414</v>
       </c>
-      <c r="H53" s="13">
+      <c r="H54" s="13">
         <v>20</v>
       </c>
-      <c r="I53" s="21">
+      <c r="I54" s="21">
         <f t="shared" si="8"/>
         <v>65.62</v>
       </c>
-      <c r="J53" s="134" t="s">
+      <c r="J54" s="134" t="s">
         <v>414</v>
       </c>
-      <c r="K53" s="148">
+      <c r="K54" s="148">
         <v>16</v>
       </c>
-      <c r="L53" s="30">
+      <c r="L54" s="30">
         <f t="shared" si="6"/>
         <v>52.496000000000002</v>
       </c>
-      <c r="M53" s="150" t="s">
+      <c r="M54" s="150" t="s">
         <v>414</v>
       </c>
-      <c r="N53" s="15">
+      <c r="N54" s="15">
         <f t="shared" si="7"/>
         <v>181.40225590551179</v>
       </c>
-      <c r="O53" s="1" t="s">
+      <c r="O54" s="1" t="s">
         <v>422</v>
       </c>
-      <c r="P53" s="130" t="s">
+      <c r="P54" s="130" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="54" spans="1:17" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="131" t="s">
+    <row r="55" spans="1:17" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A55" s="131" t="s">
         <v>116</v>
       </c>
-      <c r="B54" s="134" t="s">
+      <c r="B55" s="134" t="s">
         <v>55</v>
       </c>
-      <c r="C54" s="129">
+      <c r="C55" s="129">
         <v>36.145916999999997</v>
       </c>
-      <c r="D54" s="129">
+      <c r="D55" s="129">
         <v>-86.802161999999996</v>
       </c>
-      <c r="E54" s="26" t="s">
+      <c r="E55" s="26" t="s">
         <v>70</v>
       </c>
-      <c r="F54" s="26">
+      <c r="F55" s="26">
         <f t="shared" si="5"/>
         <v>37.00787401574803</v>
       </c>
-      <c r="G54" s="145" t="s">
+      <c r="G55" s="145" t="s">
         <v>104</v>
       </c>
-      <c r="H54" s="13">
+      <c r="H55" s="13">
         <v>15.5</v>
       </c>
-      <c r="I54" s="21">
+      <c r="I55" s="21">
         <f t="shared" si="8"/>
         <v>50.855499999999999</v>
       </c>
-      <c r="J54" s="150" t="s">
+      <c r="J55" s="150" t="s">
         <v>414</v>
       </c>
-      <c r="K54" s="159">
+      <c r="K55" s="159">
         <v>15.5</v>
       </c>
-      <c r="L54" s="161">
+      <c r="L55" s="161">
         <f t="shared" si="6"/>
         <v>50.855499999999999</v>
       </c>
-      <c r="M54" s="150" t="s">
+      <c r="M55" s="150" t="s">
         <v>414</v>
       </c>
-      <c r="N54" s="15">
+      <c r="N55" s="15">
         <f t="shared" si="7"/>
         <v>179.83294192913385</v>
       </c>
-      <c r="O54" s="131" t="s">
+      <c r="O55" s="131" t="s">
         <v>114</v>
       </c>
-      <c r="P54" s="131" t="s">
+      <c r="P55" s="131" t="s">
         <v>34</v>
       </c>
-      <c r="Q54" s="6"/>
-    </row>
-    <row r="55" spans="1:17" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="130" t="s">
+      <c r="Q55" s="6"/>
+    </row>
+    <row r="56" spans="1:17" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="130" t="s">
         <v>191</v>
       </c>
-      <c r="B55" s="134" t="s">
+      <c r="B56" s="134" t="s">
         <v>55</v>
       </c>
-      <c r="C55" s="129">
+      <c r="C56" s="129">
         <v>36.142820999999998</v>
       </c>
-      <c r="D55" s="129">
+      <c r="D56" s="129">
         <v>-86.798294999999996</v>
       </c>
-      <c r="E55" s="26" t="s">
+      <c r="E56" s="26" t="s">
         <v>190</v>
       </c>
-      <c r="F55" s="26">
+      <c r="F56" s="26">
         <f t="shared" si="5"/>
         <v>33.85826771653543</v>
       </c>
-      <c r="G55" s="24" t="s">
+      <c r="G56" s="24" t="s">
         <v>128</v>
       </c>
-      <c r="H55" s="13">
+      <c r="H56" s="13">
         <v>16.3</v>
       </c>
-      <c r="I55" s="21">
+      <c r="I56" s="21">
         <f t="shared" si="8"/>
         <v>53.480300000000007</v>
       </c>
-      <c r="J55" s="7" t="s">
+      <c r="J56" s="7" t="s">
         <v>403</v>
       </c>
-      <c r="K55" s="148">
+      <c r="K56" s="148">
         <v>15.6</v>
       </c>
-      <c r="L55" s="149">
+      <c r="L56" s="149">
         <f t="shared" si="6"/>
         <v>51.183599999999998</v>
       </c>
-      <c r="M55" s="147" t="s">
+      <c r="M56" s="147" t="s">
         <v>403</v>
       </c>
-      <c r="N55" s="15">
+      <c r="N56" s="15">
         <f t="shared" si="7"/>
         <v>172.64499527559053</v>
       </c>
-      <c r="O55" s="130" t="s">
+      <c r="O56" s="130" t="s">
         <v>187</v>
       </c>
-      <c r="P55" t="s">
+      <c r="P56" t="s">
         <v>410</v>
       </c>
-      <c r="Q55" s="6"/>
-    </row>
-    <row r="56" spans="1:17" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="7" t="s">
+      <c r="Q56" s="6"/>
+    </row>
+    <row r="57" spans="1:17" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A57" s="7" t="s">
         <v>284</v>
       </c>
-      <c r="B56" s="10" t="s">
+      <c r="B57" s="10" t="s">
         <v>285</v>
       </c>
-      <c r="C56" s="129">
+      <c r="C57" s="129">
         <v>36.145698000000003</v>
       </c>
-      <c r="D56" s="129">
+      <c r="D57" s="129">
         <v>-86.802318</v>
       </c>
-      <c r="E56" s="26" t="s">
+      <c r="E57" s="26" t="s">
         <v>286</v>
       </c>
-      <c r="F56" s="26">
+      <c r="F57" s="26">
         <f t="shared" si="5"/>
         <v>29.724409448818896</v>
       </c>
-      <c r="G56" s="24" t="s">
+      <c r="G57" s="24" t="s">
         <v>272</v>
       </c>
-      <c r="H56" s="156">
+      <c r="H57" s="156">
         <v>19.600000000000001</v>
       </c>
-      <c r="I56" s="21">
+      <c r="I57" s="21">
         <f t="shared" si="8"/>
         <v>64.307600000000008</v>
       </c>
-      <c r="J56" s="131" t="s">
+      <c r="J57" s="131" t="s">
         <v>401</v>
       </c>
-      <c r="K56" s="158">
+      <c r="K57" s="158">
         <v>16</v>
       </c>
-      <c r="L56" s="160">
+      <c r="L57" s="160">
         <f t="shared" si="6"/>
         <v>52.496000000000002</v>
       </c>
-      <c r="M56" s="157" t="s">
+      <c r="M57" s="157" t="s">
         <v>401</v>
       </c>
-      <c r="N56" s="15">
+      <c r="N57" s="15">
         <f t="shared" si="7"/>
         <v>170.81350748031494</v>
       </c>
-      <c r="O56" s="7" t="s">
+      <c r="O57" s="7" t="s">
         <v>287</v>
       </c>
-      <c r="P56" s="129" t="s">
+      <c r="P57" s="129" t="s">
         <v>374</v>
       </c>
-      <c r="Q56" s="6"/>
-    </row>
-    <row r="57" spans="1:17" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="130" t="s">
+      <c r="Q57" s="6"/>
+    </row>
+    <row r="58" spans="1:17" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A58" s="130" t="s">
         <v>278</v>
       </c>
-      <c r="B57" s="44" t="s">
+      <c r="B58" s="44" t="s">
         <v>55</v>
       </c>
-      <c r="C57" s="129">
+      <c r="C58" s="129">
         <v>36.147545999999998</v>
       </c>
-      <c r="D57" s="129">
+      <c r="D58" s="129">
         <v>-86.802178999999995</v>
       </c>
-      <c r="E57" s="48">
+      <c r="E58" s="48">
         <v>71</v>
       </c>
-      <c r="F57" s="48">
+      <c r="F58" s="48">
         <f t="shared" si="5"/>
         <v>27.952755905511811</v>
       </c>
-      <c r="G57" s="47" t="s">
+      <c r="G58" s="47" t="s">
         <v>414</v>
       </c>
-      <c r="H57" s="45">
+      <c r="H58" s="45">
         <v>20.5</v>
       </c>
-      <c r="I57" s="46">
+      <c r="I58" s="46">
         <f t="shared" si="8"/>
         <v>67.260500000000008</v>
       </c>
-      <c r="J57" s="44" t="s">
+      <c r="J58" s="44" t="s">
         <v>414</v>
       </c>
-      <c r="K57" s="49">
+      <c r="K58" s="49">
         <v>18</v>
       </c>
-      <c r="L57" s="50">
+      <c r="L58" s="50">
         <f t="shared" si="6"/>
         <v>59.058</v>
       </c>
-      <c r="M57" s="150" t="s">
+      <c r="M58" s="150" t="s">
         <v>414</v>
       </c>
-      <c r="N57" s="144">
+      <c r="N58" s="144">
         <f t="shared" si="7"/>
         <v>169.84109842519683</v>
       </c>
-      <c r="O57" s="130" t="s">
+      <c r="O58" s="130" t="s">
         <v>279</v>
       </c>
-      <c r="P57" s="130" t="s">
+      <c r="P58" s="130" t="s">
         <v>34</v>
       </c>
-      <c r="Q57" s="6"/>
-    </row>
-    <row r="58" spans="1:17" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="130" t="s">
+      <c r="Q58" s="6"/>
+    </row>
+    <row r="59" spans="1:17" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A59" s="130" t="s">
         <v>107</v>
       </c>
-      <c r="B58" s="130" t="s">
+      <c r="B59" s="130" t="s">
         <v>55</v>
       </c>
-      <c r="C58" s="51">
+      <c r="C59" s="51">
         <v>36.145654</v>
       </c>
-      <c r="D58" s="51">
+      <c r="D59" s="51">
         <v>-86.801035999999996</v>
       </c>
-      <c r="E58" s="57" t="s">
+      <c r="E59" s="57" t="s">
         <v>105</v>
       </c>
-      <c r="F58" s="57">
+      <c r="F59" s="57">
         <f t="shared" si="5"/>
         <v>34.251968503937007</v>
       </c>
-      <c r="G58" s="56" t="s">
+      <c r="G59" s="56" t="s">
         <v>104</v>
       </c>
-      <c r="H58" s="53">
+      <c r="H59" s="53">
         <v>13</v>
       </c>
-      <c r="I58" s="55">
+      <c r="I59" s="55">
         <f t="shared" si="8"/>
         <v>42.652999999999999</v>
       </c>
-      <c r="J58" s="52" t="s">
+      <c r="J59" s="52" t="s">
         <v>414</v>
       </c>
-      <c r="K58" s="58">
+      <c r="K59" s="58">
         <v>17.5</v>
       </c>
-      <c r="L58" s="59">
+      <c r="L59" s="59">
         <f t="shared" si="6"/>
         <v>57.417500000000004</v>
       </c>
-      <c r="M58" s="60" t="s">
+      <c r="M59" s="60" t="s">
         <v>414</v>
       </c>
-      <c r="N58" s="54">
+      <c r="N59" s="54">
         <f t="shared" si="7"/>
         <v>164.61301673228346</v>
       </c>
-      <c r="O58" s="130" t="s">
+      <c r="O59" s="130" t="s">
         <v>106</v>
       </c>
-      <c r="P58" s="130" t="s">
+      <c r="P59" s="130" t="s">
         <v>34</v>
       </c>
-      <c r="Q58" s="6"/>
-    </row>
-    <row r="59" spans="1:17" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="7" t="s">
+      <c r="Q59" s="6"/>
+    </row>
+    <row r="60" spans="1:17" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A60" s="7" t="s">
         <v>267</v>
       </c>
-      <c r="B59" s="137" t="s">
+      <c r="B60" s="137" t="s">
         <v>266</v>
       </c>
-      <c r="C59" s="136">
+      <c r="C60" s="136">
         <v>36.143526999999999</v>
       </c>
-      <c r="D59" s="136">
+      <c r="D60" s="136">
         <v>-86.802790999999999</v>
       </c>
-      <c r="E59" s="26" t="s">
+      <c r="E60" s="26" t="s">
         <v>265</v>
       </c>
-      <c r="F59" s="26">
+      <c r="F60" s="26">
         <f t="shared" si="5"/>
         <v>28.346456692913385</v>
       </c>
-      <c r="G59" s="24" t="s">
+      <c r="G60" s="24" t="s">
         <v>244</v>
       </c>
-      <c r="H59" s="156">
+      <c r="H60" s="156">
         <v>17.8</v>
       </c>
-      <c r="I59" s="21">
+      <c r="I60" s="21">
         <f t="shared" si="8"/>
         <v>58.401800000000001</v>
       </c>
-      <c r="J59" s="131" t="s">
+      <c r="J60" s="131" t="s">
         <v>401</v>
       </c>
-      <c r="K59" s="158">
+      <c r="K60" s="158">
         <v>19</v>
       </c>
-      <c r="L59" s="160">
+      <c r="L60" s="160">
         <f t="shared" si="6"/>
         <v>62.339000000000006</v>
       </c>
-      <c r="M59" s="157" t="s">
+      <c r="M60" s="157" t="s">
         <v>401</v>
       </c>
-      <c r="N59" s="15">
+      <c r="N60" s="15">
         <f t="shared" si="7"/>
         <v>163.03949488188977</v>
       </c>
-      <c r="O59" s="7" t="s">
+      <c r="O60" s="7" t="s">
         <v>245</v>
       </c>
-      <c r="P59" t="s">
+      <c r="P60" t="s">
         <v>376</v>
       </c>
-      <c r="Q59" s="6"/>
-    </row>
-    <row r="60" spans="1:17" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="131" t="s">
+      <c r="Q60" s="6"/>
+    </row>
+    <row r="61" spans="1:17" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A61" s="131" t="s">
         <v>379</v>
       </c>
-      <c r="B60" s="1" t="s">
+      <c r="B61" s="1" t="s">
         <v>380</v>
       </c>
-      <c r="C60">
+      <c r="C61">
         <v>36.147074000000003</v>
       </c>
-      <c r="D60">
+      <c r="D61">
         <v>-86.801820000000006</v>
       </c>
-      <c r="E60" s="26">
+      <c r="E61" s="26">
         <v>69.53</v>
       </c>
-      <c r="F60" s="26">
+      <c r="F61" s="26">
         <f t="shared" si="5"/>
         <v>27.374015748031496</v>
       </c>
-      <c r="G60" s="150" t="s">
+      <c r="G61" s="150" t="s">
         <v>377</v>
       </c>
-      <c r="H60" s="13">
+      <c r="H61" s="13">
         <v>15.6058</v>
       </c>
-      <c r="I60" s="21">
+      <c r="I61" s="21">
         <f t="shared" si="8"/>
         <v>51.202629800000004</v>
       </c>
-      <c r="J60" s="7" t="s">
+      <c r="J61" s="7" t="s">
         <v>377</v>
       </c>
-      <c r="K60" s="29">
+      <c r="K61" s="29">
         <v>15.54</v>
       </c>
-      <c r="L60" s="30">
+      <c r="L61" s="30">
         <f t="shared" si="6"/>
         <v>50.986739999999998</v>
       </c>
-      <c r="M60" s="150" t="s">
+      <c r="M61" s="150" t="s">
         <v>377</v>
       </c>
-      <c r="N60" s="15">
+      <c r="N61" s="15">
         <f t="shared" si="7"/>
         <v>149.94724893385825</v>
       </c>
-      <c r="O60" s="1" t="s">
+      <c r="O61" s="1" t="s">
         <v>392</v>
       </c>
-      <c r="P60" s="130" t="s">
+      <c r="P61" s="130" t="s">
         <v>34</v>
       </c>
-      <c r="Q60" s="6"/>
-    </row>
-    <row r="61" spans="1:17" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="134" t="s">
+      <c r="Q61" s="6"/>
+    </row>
+    <row r="62" spans="1:17" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="134" t="s">
         <v>423</v>
       </c>
-      <c r="B61" s="130" t="s">
+      <c r="B62" s="130" t="s">
         <v>55</v>
       </c>
-      <c r="C61">
+      <c r="C62">
         <v>36.148497999999996</v>
       </c>
-      <c r="D61">
+      <c r="D62">
         <v>-86.802300000000002</v>
       </c>
-      <c r="E61" s="26">
+      <c r="E62" s="26">
         <v>67</v>
       </c>
-      <c r="F61" s="26">
+      <c r="F62" s="26">
         <f t="shared" si="5"/>
         <v>26.377952755905511</v>
       </c>
-      <c r="G61" s="150" t="s">
+      <c r="G62" s="150" t="s">
         <v>414</v>
       </c>
-      <c r="H61" s="13">
+      <c r="H62" s="13">
         <v>17</v>
       </c>
-      <c r="I61" s="21">
+      <c r="I62" s="21">
         <f t="shared" si="8"/>
         <v>55.777000000000001</v>
       </c>
-      <c r="J61" s="7" t="s">
+      <c r="J62" s="7" t="s">
         <v>414</v>
       </c>
-      <c r="K61" s="29">
+      <c r="K62" s="29">
         <v>13</v>
       </c>
-      <c r="L61" s="30">
+      <c r="L62" s="30">
         <f t="shared" si="6"/>
         <v>42.652999999999999</v>
       </c>
-      <c r="M61" s="150" t="s">
+      <c r="M62" s="150" t="s">
         <v>414</v>
       </c>
-      <c r="N61" s="15">
+      <c r="N62" s="15">
         <f t="shared" si="7"/>
         <v>149.30896259842518</v>
       </c>
-      <c r="O61" s="1" t="s">
+      <c r="O62" s="1" t="s">
         <v>424</v>
       </c>
-      <c r="P61" s="1" t="s">
+      <c r="P62" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="Q61" s="6"/>
-    </row>
-    <row r="62" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A62" s="133" t="s">
+      <c r="Q62" s="6"/>
+    </row>
+    <row r="63" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A63" s="133" t="s">
         <v>382</v>
       </c>
-      <c r="B62" s="1" t="s">
+      <c r="B63" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="C62" s="130" t="s">
+      <c r="C63" s="130" t="s">
         <v>386</v>
       </c>
-      <c r="D62" s="130" t="s">
+      <c r="D63" s="130" t="s">
         <v>387</v>
       </c>
-      <c r="E62" s="26">
+      <c r="E63" s="26">
         <v>58</v>
       </c>
-      <c r="F62" s="26">
+      <c r="F63" s="26">
         <f t="shared" si="5"/>
         <v>22.834645669291337</v>
       </c>
-      <c r="G62" s="150" t="s">
+      <c r="G63" s="150" t="s">
         <v>414</v>
       </c>
-      <c r="H62" s="141">
+      <c r="H63" s="141">
         <v>19</v>
       </c>
-      <c r="I62" s="21">
+      <c r="I63" s="21">
         <f t="shared" si="8"/>
         <v>62.339000000000006</v>
       </c>
-      <c r="J62" s="7" t="s">
+      <c r="J63" s="7" t="s">
         <v>414</v>
       </c>
-      <c r="K62" s="29">
+      <c r="K63" s="29">
         <v>17.75</v>
       </c>
-      <c r="L62" s="30">
+      <c r="L63" s="30">
         <f t="shared" si="6"/>
         <v>58.237750000000005</v>
       </c>
-      <c r="M62" s="150" t="s">
+      <c r="M63" s="150" t="s">
         <v>414</v>
       </c>
-      <c r="N62" s="144">
+      <c r="N63" s="144">
         <f t="shared" si="7"/>
         <v>148.63553198818897</v>
       </c>
-      <c r="O62" s="1" t="s">
+      <c r="O63" s="1" t="s">
         <v>394</v>
       </c>
-      <c r="P62" s="130" t="s">
+      <c r="P63" s="130" t="s">
         <v>400</v>
       </c>
     </row>
-    <row r="63" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A63" s="130" t="s">
+    <row r="64" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A64" s="130" t="s">
         <v>188</v>
       </c>
-      <c r="B63" s="134" t="s">
+      <c r="B64" s="134" t="s">
         <v>55</v>
       </c>
-      <c r="C63" s="129">
+      <c r="C64" s="129">
         <v>36.142907000000001</v>
       </c>
-      <c r="D63" s="129">
+      <c r="D64" s="129">
         <v>-86.798353000000006</v>
       </c>
-      <c r="E63" s="26" t="s">
+      <c r="E64" s="26" t="s">
         <v>189</v>
       </c>
-      <c r="F63" s="26">
+      <c r="F64" s="26">
         <f t="shared" si="5"/>
         <v>24.606299212598426</v>
       </c>
-      <c r="G63" s="145" t="s">
+      <c r="G64" s="145" t="s">
         <v>128</v>
       </c>
-      <c r="H63" s="13">
+      <c r="H64" s="13">
         <v>16.2</v>
       </c>
-      <c r="I63" s="21">
+      <c r="I64" s="21">
         <f t="shared" si="8"/>
         <v>53.152200000000001</v>
       </c>
-      <c r="J63" s="7" t="s">
+      <c r="J64" s="7" t="s">
         <v>403</v>
       </c>
-      <c r="K63" s="29">
+      <c r="K64" s="29">
         <v>14.75</v>
       </c>
-      <c r="L63" s="30">
+      <c r="L64" s="30">
         <f t="shared" si="6"/>
         <v>48.394750000000002</v>
       </c>
-      <c r="M63" s="27" t="s">
+      <c r="M64" s="27" t="s">
         <v>403</v>
       </c>
-      <c r="N63" s="15">
+      <c r="N64" s="15">
         <f t="shared" si="7"/>
         <v>142.55379104330709</v>
       </c>
-      <c r="O63" s="130" t="s">
+      <c r="O64" s="130" t="s">
         <v>337</v>
       </c>
-      <c r="P63" t="s">
+      <c r="P64" t="s">
         <v>411</v>
       </c>
     </row>
-    <row r="64" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A64" s="7" t="s">
+    <row r="65" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A65" s="7" t="s">
         <v>425</v>
       </c>
-      <c r="B64" s="130" t="s">
+      <c r="B65" s="130" t="s">
         <v>55</v>
       </c>
-      <c r="C64">
+      <c r="C65">
         <v>36.148297999999997</v>
       </c>
-      <c r="D64">
+      <c r="D65">
         <v>-86.802287000000007</v>
       </c>
-      <c r="E64" s="26">
+      <c r="E65" s="26">
         <v>61</v>
       </c>
-      <c r="F64" s="26">
+      <c r="F65" s="26">
         <f t="shared" si="5"/>
         <v>24.015748031496063</v>
       </c>
-      <c r="G64" s="150" t="s">
+      <c r="G65" s="150" t="s">
         <v>414</v>
       </c>
-      <c r="H64" s="13">
+      <c r="H65" s="13">
         <v>12.5</v>
       </c>
-      <c r="I64" s="21">
+      <c r="I65" s="21">
         <f t="shared" si="8"/>
         <v>41.012500000000003</v>
       </c>
-      <c r="J64" s="7" t="s">
+      <c r="J65" s="7" t="s">
         <v>414</v>
       </c>
-      <c r="K64" s="29">
+      <c r="K65" s="29">
         <v>14.5</v>
       </c>
-      <c r="L64" s="30">
+      <c r="L65" s="30">
         <f t="shared" si="6"/>
         <v>47.5745</v>
       </c>
-      <c r="M64" s="134" t="s">
+      <c r="M65" s="134" t="s">
         <v>414</v>
       </c>
-      <c r="N64" s="15">
+      <c r="N65" s="15">
         <f t="shared" si="7"/>
         <v>128.35375885826772</v>
       </c>
-      <c r="O64" s="130" t="s">
+      <c r="O65" s="130" t="s">
         <v>426</v>
       </c>
-      <c r="P64" s="130" t="s">
+      <c r="P65" s="130" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="65" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A65" s="162" t="s">
+    <row r="66" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A66" s="162" t="s">
         <v>406</v>
       </c>
-      <c r="B65" s="138" t="s">
+      <c r="B66" s="138" t="s">
         <v>404</v>
       </c>
-      <c r="C65" s="163">
+      <c r="C66" s="163">
         <v>36.143264000000002</v>
       </c>
-      <c r="D65" s="163">
+      <c r="D66" s="163">
         <v>-86.798715000000001</v>
       </c>
-      <c r="E65" s="26">
+      <c r="E66" s="26">
         <v>32</v>
       </c>
-      <c r="F65" s="26">
+      <c r="F66" s="26">
         <f t="shared" si="5"/>
         <v>12.598425196850393</v>
       </c>
-      <c r="G65" s="150" t="s">
+      <c r="G66" s="150" t="s">
         <v>405</v>
       </c>
-      <c r="H65" s="13">
+      <c r="H66" s="13">
         <v>6.6</v>
       </c>
-      <c r="I65" s="21">
+      <c r="I66" s="21">
         <f t="shared" si="8"/>
         <v>21.654599999999999</v>
       </c>
-      <c r="J65" s="134" t="s">
+      <c r="J66" s="134" t="s">
         <v>405</v>
       </c>
-      <c r="K65" s="148">
+      <c r="K66" s="148">
         <v>8.85</v>
       </c>
-      <c r="L65" s="149">
+      <c r="L66" s="149">
         <f t="shared" si="6"/>
         <v>29.036850000000001</v>
       </c>
-      <c r="M65" s="150" t="s">
+      <c r="M66" s="150" t="s">
         <v>405</v>
       </c>
-      <c r="N65" s="15">
+      <c r="N66" s="15">
         <f t="shared" si="7"/>
         <v>68.492899114173227</v>
       </c>
-      <c r="O65" s="1" t="s">
+      <c r="O66" s="1" t="s">
         <v>408</v>
       </c>
-      <c r="P65" s="1" t="s">
+      <c r="P66" s="1" t="s">
         <v>407</v>
-      </c>
-    </row>
-    <row r="66" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A66" s="131" t="s">
-        <v>56</v>
-      </c>
-      <c r="B66" s="131" t="s">
-        <v>55</v>
-      </c>
-      <c r="C66" s="132">
-        <v>36.146718</v>
-      </c>
-      <c r="D66" s="132">
-        <v>-86.802537000000001</v>
-      </c>
-      <c r="E66" s="26" t="s">
-        <v>77</v>
-      </c>
-      <c r="F66" s="26">
-        <f t="shared" si="5"/>
-        <v>46.45669291338583</v>
-      </c>
-      <c r="G66" s="24" t="s">
-        <v>104</v>
-      </c>
-      <c r="H66" s="13"/>
-      <c r="I66" s="21">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="J66" s="7"/>
-      <c r="K66" s="29"/>
-      <c r="L66" s="30">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="N66" s="15">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="O66" s="131" t="s">
-        <v>89</v>
-      </c>
-      <c r="P66" s="129" t="s">
-        <v>360</v>
       </c>
     </row>
     <row r="67" spans="1:17" x14ac:dyDescent="0.25">
@@ -7077,7 +7081,7 @@
       </c>
       <c r="H79" s="13"/>
       <c r="I79" s="21">
-        <f t="shared" ref="I79:I110" si="12">H79*3.281</f>
+        <f t="shared" ref="I79:I109" si="12">H79*3.281</f>
         <v>0</v>
       </c>
       <c r="J79" s="7"/>
@@ -8031,7 +8035,7 @@
         <v>82</v>
       </c>
       <c r="F100" s="26">
-        <f t="shared" ref="F100:F131" si="13">E100/2.54</f>
+        <f t="shared" ref="F100:F109" si="13">E100/2.54</f>
         <v>32.677165354330711</v>
       </c>
       <c r="G100" s="151" t="s">
@@ -8045,7 +8049,7 @@
       <c r="J100" s="7"/>
       <c r="K100" s="29"/>
       <c r="L100" s="30">
-        <f t="shared" ref="L100:L131" si="14">K100*3.281</f>
+        <f t="shared" ref="L100:L109" si="14">K100*3.281</f>
         <v>0</v>
       </c>
       <c r="N100" s="15">
@@ -22411,7 +22415,7 @@
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="str">
-        <f>primary!A45</f>
+        <f>primary!A46</f>
         <v>2-185</v>
       </c>
       <c r="B31" s="1" t="str">
@@ -22495,337 +22499,337 @@
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="str">
-        <f>primary!A37</f>
+        <f>primary!A38</f>
         <v>4-943</v>
       </c>
       <c r="B33" s="1" t="str">
-        <f>primary!B37</f>
+        <f>primary!B38</f>
         <v>Magnolia grandiflora</v>
       </c>
       <c r="C33" s="1">
-        <f>primary!C37</f>
+        <f>primary!C38</f>
         <v>36.145836000000003</v>
       </c>
       <c r="D33" s="1">
-        <f>primary!D37</f>
+        <f>primary!D38</f>
         <v>-86.802235999999994</v>
       </c>
       <c r="E33" s="1" t="str">
-        <f>primary!E37</f>
+        <f>primary!E38</f>
         <v>109</v>
       </c>
       <c r="F33" s="14">
-        <f>primary!H37</f>
+        <f>primary!H38</f>
         <v>22.005486132276744</v>
       </c>
       <c r="G33" s="1">
-        <f>primary!K37</f>
+        <f>primary!K38</f>
         <v>19</v>
       </c>
       <c r="H33" s="22">
-        <f>primary!N37</f>
+        <f>primary!N38</f>
         <v>222.60101377952756</v>
       </c>
       <c r="I33" s="1" t="str">
-        <f>primary!O37</f>
+        <f>primary!O38</f>
         <v>front Buttrick, s. of entry walk</v>
       </c>
       <c r="J33" s="1" t="str">
-        <f>primary!P37</f>
+        <f>primary!P38</f>
         <v>http://bioimages.vanderbilt.edu/vanderbilt/7-23</v>
       </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="str">
-        <f>primary!A38</f>
+        <f>primary!A39</f>
         <v>2-780</v>
       </c>
       <c r="B34" s="1" t="str">
-        <f>primary!B38</f>
+        <f>primary!B39</f>
         <v>Liriodendron tulipifera</v>
       </c>
       <c r="C34" s="1">
-        <f>primary!C38</f>
+        <f>primary!C39</f>
         <v>36.147970000000001</v>
       </c>
       <c r="D34" s="1">
-        <f>primary!D38</f>
+        <f>primary!D39</f>
         <v>-86.802019000000001</v>
       </c>
       <c r="E34" s="1" t="str">
-        <f>primary!E38</f>
+        <f>primary!E39</f>
         <v>104</v>
       </c>
       <c r="F34" s="14">
-        <f>primary!H38</f>
+        <f>primary!H39</f>
         <v>23.67</v>
       </c>
       <c r="G34" s="1">
-        <f>primary!K38</f>
+        <f>primary!K39</f>
         <v>17.07</v>
       </c>
       <c r="H34" s="22">
-        <f>primary!N38</f>
+        <f>primary!N39</f>
         <v>220.29496899606298</v>
       </c>
       <c r="I34" s="1" t="str">
-        <f>primary!O38</f>
+        <f>primary!O39</f>
         <v>Between Kirkland and Furman Halls</v>
       </c>
       <c r="J34" s="1" t="str">
-        <f>primary!P38</f>
+        <f>primary!P39</f>
         <v>http://bioimages.vanderbilt.edu/vanderbilt/3-4</v>
       </c>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="str">
-        <f>primary!A39</f>
+        <f>primary!A40</f>
         <v>2-528</v>
       </c>
       <c r="B35" s="1" t="str">
-        <f>primary!B39</f>
+        <f>primary!B40</f>
         <v>Ulmus serotina</v>
       </c>
       <c r="C35" s="1">
-        <f>primary!C39</f>
+        <f>primary!C40</f>
         <v>36.146864000000001</v>
       </c>
       <c r="D35" s="1">
-        <f>primary!D39</f>
+        <f>primary!D40</f>
         <v>-86.801839000000001</v>
       </c>
       <c r="E35" s="1" t="str">
-        <f>primary!E39</f>
+        <f>primary!E40</f>
         <v>83</v>
       </c>
       <c r="F35" s="14">
-        <f>primary!H39</f>
+        <f>primary!H40</f>
         <v>28.649801889667781</v>
       </c>
       <c r="G35" s="1">
-        <f>primary!K39</f>
+        <f>primary!K40</f>
         <v>20.5</v>
       </c>
       <c r="H35" s="22">
-        <f>primary!N39</f>
+        <f>primary!N40</f>
         <v>213.47338090551179</v>
       </c>
       <c r="I35" s="1" t="str">
-        <f>primary!O39</f>
+        <f>primary!O40</f>
         <v>Between Benson Hall and Garland Hall</v>
       </c>
       <c r="J35" s="1" t="str">
-        <f>primary!P39</f>
+        <f>primary!P40</f>
         <v>http://bioimages.vanderbilt.edu/vanderbilt/7-340</v>
       </c>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="str">
-        <f>primary!A40</f>
+        <f>primary!A41</f>
         <v>2-247</v>
       </c>
       <c r="B36" s="1" t="str">
-        <f>primary!B40</f>
+        <f>primary!B41</f>
         <v>Magnolia grandiflora</v>
       </c>
       <c r="C36" s="1">
-        <f>primary!C40</f>
+        <f>primary!C41</f>
         <v>36.145913999999998</v>
       </c>
       <c r="D36" s="1">
-        <f>primary!D40</f>
+        <f>primary!D41</f>
         <v>-86.801046999999997</v>
       </c>
       <c r="E36" s="1" t="str">
-        <f>primary!E40</f>
+        <f>primary!E41</f>
         <v>110</v>
       </c>
       <c r="F36" s="14">
-        <f>primary!H40</f>
+        <f>primary!H41</f>
         <v>18.5</v>
       </c>
       <c r="G36" s="1">
-        <f>primary!K40</f>
+        <f>primary!K41</f>
         <v>17.75</v>
       </c>
       <c r="H36" s="22">
-        <f>primary!N40</f>
+        <f>primary!N41</f>
         <v>211.31104773622047</v>
       </c>
       <c r="I36" s="1" t="str">
-        <f>primary!O40</f>
+        <f>primary!O41</f>
         <v>in front of central library veering north</v>
       </c>
       <c r="J36" s="1" t="str">
-        <f>primary!P40</f>
+        <f>primary!P41</f>
         <v>http://bioimages.vanderbilt.edu/vanderbilt/6-143</v>
       </c>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="str">
-        <f>primary!A41</f>
+        <f>primary!A42</f>
         <v>2-182</v>
       </c>
       <c r="B37" s="1" t="str">
-        <f>primary!B41</f>
+        <f>primary!B42</f>
         <v>Catalpa speciosa</v>
       </c>
       <c r="C37" s="1">
-        <f>primary!C41</f>
+        <f>primary!C42</f>
         <v>36.146563999999998</v>
       </c>
       <c r="D37" s="1">
-        <f>primary!D41</f>
+        <f>primary!D42</f>
         <v>-86.801297000000005</v>
       </c>
       <c r="E37" s="1" t="str">
-        <f>primary!E41</f>
+        <f>primary!E42</f>
         <v>111</v>
       </c>
       <c r="F37" s="14">
-        <f>primary!H41</f>
+        <f>primary!H42</f>
         <v>18.40902163974398</v>
       </c>
       <c r="G37" s="1">
-        <f>primary!K41</f>
+        <f>primary!K42</f>
         <v>16</v>
       </c>
       <c r="H37" s="22">
-        <f>primary!N41</f>
+        <f>primary!N42</f>
         <v>210.81395669291337</v>
       </c>
       <c r="I37" s="1" t="str">
-        <f>primary!O41</f>
+        <f>primary!O42</f>
         <v>Between the Divinity School and Garland Hall</v>
       </c>
       <c r="J37" s="1" t="str">
-        <f>primary!P41</f>
+        <f>primary!P42</f>
         <v>http://bioimages.vanderbilt.edu/vanderbilt/6-159</v>
       </c>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="str">
-        <f>primary!A42</f>
+        <f>primary!A43</f>
         <v>2-663</v>
       </c>
       <c r="B38" s="1" t="str">
-        <f>primary!B42</f>
+        <f>primary!B43</f>
         <v>Magnolia grandiflora</v>
       </c>
       <c r="C38" s="1">
-        <f>primary!C42</f>
+        <f>primary!C43</f>
         <v>36.146968000000001</v>
       </c>
       <c r="D38" s="1">
-        <f>primary!D42</f>
+        <f>primary!D43</f>
         <v>-86.801186000000001</v>
       </c>
       <c r="E38" s="1" t="str">
-        <f>primary!E42</f>
+        <f>primary!E43</f>
         <v>109</v>
       </c>
       <c r="F38" s="14">
-        <f>primary!H42</f>
+        <f>primary!H43</f>
         <v>18.5</v>
       </c>
       <c r="G38" s="1">
-        <f>primary!K42</f>
+        <f>primary!K43</f>
         <v>16</v>
       </c>
       <c r="H38" s="22">
-        <f>primary!N42</f>
+        <f>primary!N43</f>
         <v>208.63876377952755</v>
       </c>
       <c r="I38" s="1" t="str">
-        <f>primary!O42</f>
+        <f>primary!O43</f>
         <v>northeast of Bishop McTyeire's tomb; trunk splits just above measured height</v>
       </c>
       <c r="J38" s="1" t="str">
-        <f>primary!P42</f>
+        <f>primary!P43</f>
         <v>http://bioimages.vanderbilt.edu/vanderbilt/4-155</v>
       </c>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="str">
-        <f>primary!A43</f>
+        <f>primary!A44</f>
         <v>2-1002</v>
       </c>
       <c r="B39" s="1" t="str">
-        <f>primary!B43</f>
+        <f>primary!B44</f>
         <v>Magnolia grandiflora</v>
       </c>
       <c r="C39" s="1">
-        <f>primary!C43</f>
+        <f>primary!C44</f>
         <v>36.148797999999999</v>
       </c>
       <c r="D39" s="1">
-        <f>primary!D43</f>
+        <f>primary!D44</f>
         <v>-86.801866000000004</v>
       </c>
       <c r="E39" s="1">
-        <f>primary!E43</f>
+        <f>primary!E44</f>
         <v>106</v>
       </c>
       <c r="F39" s="14">
-        <f>primary!H43</f>
+        <f>primary!H44</f>
         <v>19</v>
       </c>
       <c r="G39" s="1">
-        <f>primary!K43</f>
+        <f>primary!K44</f>
         <v>17.25</v>
       </c>
       <c r="H39" s="22">
-        <f>primary!N43</f>
+        <f>primary!N44</f>
         <v>207.59403690944882</v>
       </c>
       <c r="I39" s="1" t="str">
-        <f>primary!O43</f>
+        <f>primary!O44</f>
         <v>between Kissam Dorms and Curry Field</v>
       </c>
       <c r="J39" s="1" t="str">
-        <f>primary!P43</f>
+        <f>primary!P44</f>
         <v>none</v>
       </c>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="str">
-        <f>primary!A44</f>
+        <f>primary!A45</f>
         <v>2-861</v>
       </c>
       <c r="B40" s="1" t="str">
-        <f>primary!B44</f>
+        <f>primary!B45</f>
         <v>Fraxinus americana</v>
       </c>
       <c r="C40" s="1">
-        <f>primary!C44</f>
+        <f>primary!C45</f>
         <v>36.148634000000001</v>
       </c>
       <c r="D40" s="1">
-        <f>primary!D44</f>
+        <f>primary!D45</f>
         <v>-86.801985999999999</v>
       </c>
       <c r="E40" s="1" t="str">
-        <f>primary!E44</f>
+        <f>primary!E45</f>
         <v>101</v>
       </c>
       <c r="F40" s="14">
-        <f>primary!H44</f>
+        <f>primary!H45</f>
         <v>19.5</v>
       </c>
       <c r="G40" s="1">
-        <f>primary!K44</f>
+        <f>primary!K45</f>
         <v>18</v>
       </c>
       <c r="H40" s="22">
-        <f>primary!N44</f>
+        <f>primary!N45</f>
         <v>203.66549212598426</v>
       </c>
       <c r="I40" s="1" t="str">
-        <f>primary!O44</f>
+        <f>primary!O45</f>
         <v>beteen Kirkland and Curry Field</v>
       </c>
       <c r="J40" s="1" t="str">
-        <f>primary!P44</f>
+        <f>primary!P45</f>
         <v>http://bioimages.vanderbilt.edu/vanderbilt/1-183</v>
       </c>
     </row>
@@ -22835,291 +22839,291 @@
         <v>#REF!</v>
       </c>
       <c r="B41" s="1" t="str">
-        <f>primary!B45</f>
+        <f>primary!B46</f>
         <v>Ginkgo biloba</v>
       </c>
       <c r="C41" s="1">
-        <f>primary!C45</f>
+        <f>primary!C46</f>
         <v>36.148558999999999</v>
       </c>
       <c r="D41" s="1">
-        <f>primary!D45</f>
+        <f>primary!D46</f>
         <v>-86.803090999999995</v>
       </c>
       <c r="E41" s="1" t="str">
-        <f>primary!E45</f>
+        <f>primary!E46</f>
         <v>100</v>
       </c>
       <c r="F41" s="14">
-        <f>primary!H45</f>
+        <f>primary!H46</f>
         <v>18</v>
       </c>
       <c r="G41" s="1">
-        <f>primary!K45</f>
+        <f>primary!K46</f>
         <v>23.5</v>
       </c>
       <c r="H41" s="22">
-        <f>primary!N45</f>
+        <f>primary!N46</f>
         <v>202.01852066929132</v>
       </c>
       <c r="I41" s="1" t="str">
-        <f>primary!O45</f>
+        <f>primary!O46</f>
         <v>between Kirkland and Barnard Halls; "Galloway's ginkgo"</v>
       </c>
       <c r="J41" s="1" t="str">
-        <f>primary!P45</f>
+        <f>primary!P46</f>
         <v>http://bioimages.vanderbilt.edu/vanderbilt/2-101</v>
       </c>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="str">
-        <f>primary!A46</f>
+        <f>primary!A47</f>
         <v>2-759</v>
       </c>
       <c r="B42" s="1" t="str">
-        <f>primary!B46</f>
+        <f>primary!B47</f>
         <v>Quercus alba</v>
       </c>
       <c r="C42" s="1">
-        <f>primary!C46</f>
+        <f>primary!C47</f>
         <v>36.148681000000003</v>
       </c>
       <c r="D42" s="1">
-        <f>primary!D46</f>
+        <f>primary!D47</f>
         <v>-86.802809999999994</v>
       </c>
       <c r="E42" s="1" t="str">
-        <f>primary!E46</f>
+        <f>primary!E47</f>
         <v>95</v>
       </c>
       <c r="F42" s="14">
-        <f>primary!H46</f>
+        <f>primary!H47</f>
         <v>19.597683633038706</v>
       </c>
       <c r="G42" s="1">
-        <f>primary!K46</f>
+        <f>primary!K47</f>
         <v>23</v>
       </c>
       <c r="H42" s="22">
-        <f>primary!N46</f>
+        <f>primary!N47</f>
         <v>200.66616338582676</v>
       </c>
       <c r="I42" s="1" t="str">
-        <f>primary!O46</f>
+        <f>primary!O47</f>
         <v>between Kirkland and West End Ave.</v>
       </c>
       <c r="J42" s="1" t="str">
-        <f>primary!P46</f>
+        <f>primary!P47</f>
         <v>none</v>
       </c>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="str">
-        <f>primary!A47</f>
+        <f>primary!A48</f>
         <v>2-461</v>
       </c>
       <c r="B43" s="1" t="str">
-        <f>primary!B47</f>
+        <f>primary!B48</f>
         <v>Magnolia grandiflora</v>
       </c>
       <c r="C43" s="1">
-        <f>primary!C47</f>
+        <f>primary!C48</f>
         <v>36.148344000000002</v>
       </c>
       <c r="D43" s="1">
-        <f>primary!D47</f>
+        <f>primary!D48</f>
         <v>-86.802238000000003</v>
       </c>
       <c r="E43" s="1">
-        <f>primary!E47</f>
+        <f>primary!E48</f>
         <v>107</v>
       </c>
       <c r="F43" s="14">
-        <f>primary!H47</f>
+        <f>primary!H48</f>
         <v>15</v>
       </c>
       <c r="G43" s="1">
-        <f>primary!K47</f>
+        <f>primary!K48</f>
         <v>15.25</v>
       </c>
       <c r="H43" s="22">
-        <f>primary!N47</f>
+        <f>primary!N48</f>
         <v>194.06638336614174</v>
       </c>
       <c r="I43" s="1" t="str">
-        <f>primary!O47</f>
+        <f>primary!O48</f>
         <v>east of Kirkland Hall; southwest of Kissam Quad; second tree north of curve in drive</v>
       </c>
       <c r="J43" s="1" t="str">
-        <f>primary!P47</f>
+        <f>primary!P48</f>
         <v>none</v>
       </c>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="str">
-        <f>primary!A48</f>
+        <f>primary!A49</f>
         <v>2-1006</v>
       </c>
       <c r="B44" s="1" t="str">
-        <f>primary!B48</f>
+        <f>primary!B49</f>
         <v>Fraxinus americana</v>
       </c>
       <c r="C44" s="1">
-        <f>primary!C48</f>
+        <f>primary!C49</f>
         <v>36.148788000000003</v>
       </c>
       <c r="D44" s="1">
-        <f>primary!D48</f>
+        <f>primary!D49</f>
         <v>-86.803242999999995</v>
       </c>
       <c r="E44" s="1">
-        <f>primary!E48</f>
+        <f>primary!E49</f>
         <v>95.5</v>
       </c>
       <c r="F44" s="14">
-        <f>primary!H48</f>
+        <f>primary!H49</f>
         <v>16.78</v>
       </c>
       <c r="G44" s="1">
-        <f>primary!K48</f>
+        <f>primary!K49</f>
         <v>21.25</v>
       </c>
       <c r="H44" s="22">
-        <f>primary!N48</f>
+        <f>primary!N49</f>
         <v>190.60432911417325</v>
       </c>
       <c r="I44" s="1" t="str">
-        <f>primary!O48</f>
+        <f>primary!O49</f>
         <v>next to the a/c unit, behind Barnard Hall; surrounded by shrubs and mosquitoes</v>
       </c>
       <c r="J44" s="1" t="str">
-        <f>primary!P48</f>
+        <f>primary!P49</f>
         <v>http://bioimages.vanderbilt.edu/vanderbilt/2-95</v>
       </c>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="str">
-        <f>primary!A49</f>
+        <f>primary!A50</f>
         <v>1-727</v>
       </c>
       <c r="B45" s="1" t="str">
-        <f>primary!B49</f>
+        <f>primary!B50</f>
         <v>Magnolia grandiflora</v>
       </c>
       <c r="C45" s="1">
-        <f>primary!C49</f>
+        <f>primary!C50</f>
         <v>36.142912000000003</v>
       </c>
       <c r="D45" s="1">
-        <f>primary!D49</f>
+        <f>primary!D50</f>
         <v>-86.798676</v>
       </c>
       <c r="E45" s="1" t="str">
-        <f>primary!E49</f>
+        <f>primary!E50</f>
         <v>94.5</v>
       </c>
       <c r="F45" s="14">
-        <f>primary!H49</f>
+        <f>primary!H50</f>
         <v>18.100000000000001</v>
       </c>
       <c r="G45" s="1">
-        <f>primary!K49</f>
+        <f>primary!K50</f>
         <v>13.5</v>
       </c>
       <c r="H45" s="22">
-        <f>primary!N49</f>
+        <f>primary!N50</f>
         <v>187.34146515748031</v>
       </c>
       <c r="I45" s="1" t="str">
-        <f>primary!O49</f>
+        <f>primary!O50</f>
         <v>western magnolia in Magnolia Lawn along Magnolia Circle</v>
       </c>
       <c r="J45" s="1" t="str">
-        <f>primary!P49</f>
+        <f>primary!P50</f>
         <v>http://bioimages.vanderbilt.edu/vanderbilt/12-190</v>
       </c>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="str">
-        <f>primary!A50</f>
+        <f>primary!A51</f>
         <v>2-482</v>
       </c>
       <c r="B46" s="1" t="str">
-        <f>primary!B50</f>
+        <f>primary!B51</f>
         <v>Magnolia grandiflora</v>
       </c>
       <c r="C46" s="1">
-        <f>primary!C50</f>
+        <f>primary!C51</f>
         <v>36.146942000000003</v>
       </c>
       <c r="D46" s="1">
-        <f>primary!D50</f>
+        <f>primary!D51</f>
         <v>-86.801242999999999</v>
       </c>
       <c r="E46" s="1" t="str">
-        <f>primary!E50</f>
+        <f>primary!E51</f>
         <v>85</v>
       </c>
       <c r="F46" s="14">
-        <f>primary!H50</f>
+        <f>primary!H51</f>
         <v>19</v>
       </c>
       <c r="G46" s="1">
-        <f>primary!K50</f>
+        <f>primary!K51</f>
         <v>21.25</v>
       </c>
       <c r="H46" s="22">
-        <f>primary!N50</f>
+        <f>primary!N51</f>
         <v>184.90126131889764</v>
       </c>
       <c r="I46" s="1" t="str">
-        <f>primary!O50</f>
+        <f>primary!O51</f>
         <v>northwest of Bishop McTyeire's tomb; trunk splits just above measured height</v>
       </c>
       <c r="J46" s="1" t="str">
-        <f>primary!P50</f>
+        <f>primary!P51</f>
         <v>http://bioimages.vanderbilt.edu/vanderbilt/4-156</v>
       </c>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="str">
-        <f>primary!A55</f>
+        <f>primary!A56</f>
         <v>1-731</v>
       </c>
       <c r="B47" s="1" t="str">
-        <f>primary!B55</f>
+        <f>primary!B56</f>
         <v>Magnolia grandiflora</v>
       </c>
       <c r="C47" s="1">
-        <f>primary!C55</f>
+        <f>primary!C56</f>
         <v>36.142820999999998</v>
       </c>
       <c r="D47" s="1">
-        <f>primary!D55</f>
+        <f>primary!D56</f>
         <v>-86.798294999999996</v>
       </c>
       <c r="E47" s="1" t="str">
-        <f>primary!E55</f>
+        <f>primary!E56</f>
         <v>86</v>
       </c>
       <c r="F47" s="14">
-        <f>primary!H55</f>
+        <f>primary!H56</f>
         <v>16.3</v>
       </c>
       <c r="G47" s="1">
-        <f>primary!K55</f>
+        <f>primary!K56</f>
         <v>15.6</v>
       </c>
       <c r="H47" s="22">
-        <f>primary!N55</f>
+        <f>primary!N56</f>
         <v>172.64499527559053</v>
       </c>
       <c r="I47" s="1" t="str">
-        <f>primary!O55</f>
+        <f>primary!O56</f>
         <v>southeastern magnolia in Magnolia Lawn along Magnolia Circle</v>
       </c>
       <c r="J47" s="1" t="str">
-        <f>primary!P55</f>
+        <f>primary!P56</f>
         <v>http://bioimages.vanderbilt.edu/vanderbilt/12-192</v>
       </c>
     </row>
@@ -23167,43 +23171,43 @@
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="str">
-        <f>primary!A56</f>
+        <f>primary!A57</f>
         <v>4-208</v>
       </c>
       <c r="B49" s="1" t="str">
-        <f>primary!B56</f>
+        <f>primary!B57</f>
         <v>Sophora japonica</v>
       </c>
       <c r="C49" s="1">
-        <f>primary!C56</f>
+        <f>primary!C57</f>
         <v>36.145698000000003</v>
       </c>
       <c r="D49" s="1">
-        <f>primary!D56</f>
+        <f>primary!D57</f>
         <v>-86.802318</v>
       </c>
       <c r="E49" s="1" t="str">
-        <f>primary!E56</f>
+        <f>primary!E57</f>
         <v>75.5</v>
       </c>
       <c r="F49" s="14">
-        <f>primary!H56</f>
+        <f>primary!H57</f>
         <v>19.600000000000001</v>
       </c>
       <c r="G49" s="1">
-        <f>primary!K56</f>
+        <f>primary!K57</f>
         <v>16</v>
       </c>
       <c r="H49" s="22">
-        <f>primary!N56</f>
+        <f>primary!N57</f>
         <v>170.81350748031494</v>
       </c>
       <c r="I49" s="1" t="str">
-        <f>primary!O56</f>
+        <f>primary!O57</f>
         <v>east of Buttrick Hall; former state champion</v>
       </c>
       <c r="J49" s="1" t="str">
-        <f>primary!P56</f>
+        <f>primary!P57</f>
         <v>http://bioimages.vanderbilt.edu/vanderbilt/7-29</v>
       </c>
     </row>
@@ -23251,421 +23255,421 @@
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="str">
-        <f>primary!A57</f>
+        <f>primary!A58</f>
         <v>2-865</v>
       </c>
       <c r="B51" s="1" t="str">
-        <f>primary!B57</f>
+        <f>primary!B58</f>
         <v>Magnolia grandiflora</v>
       </c>
       <c r="C51" s="1">
-        <f>primary!C57</f>
+        <f>primary!C58</f>
         <v>36.147545999999998</v>
       </c>
       <c r="D51" s="1">
-        <f>primary!D57</f>
+        <f>primary!D58</f>
         <v>-86.802178999999995</v>
       </c>
       <c r="E51" s="1">
-        <f>primary!E57</f>
+        <f>primary!E58</f>
         <v>71</v>
       </c>
       <c r="F51" s="14">
-        <f>primary!H57</f>
+        <f>primary!H58</f>
         <v>20.5</v>
       </c>
       <c r="G51" s="1">
-        <f>primary!K57</f>
+        <f>primary!K58</f>
         <v>18</v>
       </c>
       <c r="H51" s="22">
-        <f>primary!N57</f>
+        <f>primary!N58</f>
         <v>169.84109842519683</v>
       </c>
       <c r="I51" s="1" t="str">
-        <f>primary!O57</f>
+        <f>primary!O58</f>
         <v>north of Benson Hall; by Margaret Branscomb statue</v>
       </c>
       <c r="J51" s="1" t="str">
-        <f>primary!P57</f>
+        <f>primary!P58</f>
         <v>none</v>
       </c>
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="str">
-        <f>primary!A58</f>
+        <f>primary!A59</f>
         <v>2-959</v>
       </c>
       <c r="B52" s="1" t="str">
-        <f>primary!B58</f>
+        <f>primary!B59</f>
         <v>Magnolia grandiflora</v>
       </c>
       <c r="C52" s="1">
-        <f>primary!C58</f>
+        <f>primary!C59</f>
         <v>36.145654</v>
       </c>
       <c r="D52" s="1">
-        <f>primary!D58</f>
+        <f>primary!D59</f>
         <v>-86.801035999999996</v>
       </c>
       <c r="E52" s="1" t="str">
-        <f>primary!E58</f>
+        <f>primary!E59</f>
         <v>87</v>
       </c>
       <c r="F52" s="14">
-        <f>primary!H58</f>
+        <f>primary!H59</f>
         <v>13</v>
       </c>
       <c r="G52" s="1">
-        <f>primary!K58</f>
+        <f>primary!K59</f>
         <v>17.5</v>
       </c>
       <c r="H52" s="22">
-        <f>primary!N58</f>
+        <f>primary!N59</f>
         <v>164.61301673228346</v>
       </c>
       <c r="I52" s="1" t="str">
-        <f>primary!O58</f>
+        <f>primary!O59</f>
         <v>in front of central library veering south</v>
       </c>
       <c r="J52" s="1" t="str">
-        <f>primary!P58</f>
+        <f>primary!P59</f>
         <v>none</v>
       </c>
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="str">
-        <f>primary!A59</f>
+        <f>primary!A60</f>
         <v>4-616</v>
       </c>
       <c r="B53" s="1" t="str">
-        <f>primary!B59</f>
+        <f>primary!B60</f>
         <v>Juglans nigra</v>
       </c>
       <c r="C53" s="1">
-        <f>primary!C59</f>
+        <f>primary!C60</f>
         <v>36.143526999999999</v>
       </c>
       <c r="D53" s="1">
-        <f>primary!D59</f>
+        <f>primary!D60</f>
         <v>-86.802790999999999</v>
       </c>
       <c r="E53" s="1" t="str">
-        <f>primary!E59</f>
+        <f>primary!E60</f>
         <v>72</v>
       </c>
       <c r="F53" s="14">
-        <f>primary!H59</f>
+        <f>primary!H60</f>
         <v>17.8</v>
       </c>
       <c r="G53" s="1">
-        <f>primary!K59</f>
+        <f>primary!K60</f>
         <v>19</v>
       </c>
       <c r="H53" s="22">
-        <f>primary!N59</f>
+        <f>primary!N60</f>
         <v>163.03949488188977</v>
       </c>
       <c r="I53" s="1" t="str">
-        <f>primary!O59</f>
+        <f>primary!O60</f>
         <v>between McTyeire and the Round Wing</v>
       </c>
       <c r="J53" s="1" t="str">
-        <f>primary!P59</f>
+        <f>primary!P60</f>
         <v>http://bioimages.vanderbilt.edu/vanderbilt/11-221</v>
       </c>
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="str">
-        <f>primary!A60</f>
+        <f>primary!A61</f>
         <v>2-886</v>
       </c>
       <c r="B54" s="1" t="str">
-        <f>primary!B60</f>
+        <f>primary!B61</f>
         <v>Acer saccharum</v>
       </c>
       <c r="C54" s="1">
-        <f>primary!C60</f>
+        <f>primary!C61</f>
         <v>36.147074000000003</v>
       </c>
       <c r="D54" s="1">
-        <f>primary!D60</f>
+        <f>primary!D61</f>
         <v>-86.801820000000006</v>
       </c>
       <c r="E54" s="1">
-        <f>primary!E60</f>
+        <f>primary!E61</f>
         <v>69.53</v>
       </c>
       <c r="F54" s="14">
-        <f>primary!H60</f>
+        <f>primary!H61</f>
         <v>15.6058</v>
       </c>
       <c r="G54" s="1">
-        <f>primary!K60</f>
+        <f>primary!K61</f>
         <v>15.54</v>
       </c>
       <c r="H54" s="22">
-        <f>primary!N60</f>
+        <f>primary!N61</f>
         <v>149.94724893385825</v>
       </c>
       <c r="I54" s="1" t="str">
-        <f>primary!O60</f>
+        <f>primary!O61</f>
         <v>next to the left side of Benson Hall from the front</v>
       </c>
       <c r="J54" s="1" t="str">
-        <f>primary!P60</f>
+        <f>primary!P61</f>
         <v>none</v>
       </c>
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="str">
-        <f>primary!A61</f>
+        <f>primary!A62</f>
         <v>2-386</v>
       </c>
       <c r="B55" s="1" t="str">
-        <f>primary!B61</f>
+        <f>primary!B62</f>
         <v>Magnolia grandiflora</v>
       </c>
       <c r="C55" s="1">
-        <f>primary!C61</f>
+        <f>primary!C62</f>
         <v>36.148497999999996</v>
       </c>
       <c r="D55" s="1">
-        <f>primary!D61</f>
+        <f>primary!D62</f>
         <v>-86.802300000000002</v>
       </c>
       <c r="E55" s="1">
-        <f>primary!E61</f>
+        <f>primary!E62</f>
         <v>67</v>
       </c>
       <c r="F55" s="14">
-        <f>primary!H61</f>
+        <f>primary!H62</f>
         <v>17</v>
       </c>
       <c r="G55" s="1">
-        <f>primary!K61</f>
+        <f>primary!K62</f>
         <v>13</v>
       </c>
       <c r="H55" s="22">
-        <f>primary!N61</f>
+        <f>primary!N62</f>
         <v>149.30896259842518</v>
       </c>
       <c r="I55" s="1" t="str">
-        <f>primary!O61</f>
+        <f>primary!O62</f>
         <v>east of Kirkland Hall; southwest of Kissam Quad; fourth tree north of curve in drive (last one)</v>
       </c>
       <c r="J55" s="1" t="str">
-        <f>primary!P61</f>
+        <f>primary!P62</f>
         <v>none</v>
       </c>
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="str">
-        <f>primary!A62</f>
+        <f>primary!A63</f>
         <v>2-791</v>
       </c>
       <c r="B56" s="1" t="str">
-        <f>primary!B62</f>
+        <f>primary!B63</f>
         <v>Magnolia grandiflora</v>
       </c>
       <c r="C56" s="1" t="str">
-        <f>primary!C62</f>
+        <f>primary!C63</f>
         <v>36.148494</v>
       </c>
       <c r="D56" s="1" t="str">
-        <f>primary!D62</f>
+        <f>primary!D63</f>
         <v>-86.802021</v>
       </c>
       <c r="E56" s="1">
-        <f>primary!E62</f>
+        <f>primary!E63</f>
         <v>58</v>
       </c>
       <c r="F56" s="14">
-        <f>primary!H62</f>
+        <f>primary!H63</f>
         <v>19</v>
       </c>
       <c r="G56" s="1">
-        <f>primary!K62</f>
+        <f>primary!K63</f>
         <v>17.75</v>
       </c>
       <c r="H56" s="22">
-        <f>primary!N62</f>
+        <f>primary!N63</f>
         <v>148.63553198818897</v>
       </c>
       <c r="I56" s="1" t="str">
-        <f>primary!O62</f>
+        <f>primary!O63</f>
         <v>east of the drive near Kirkland Hall</v>
       </c>
       <c r="J56" s="1" t="str">
-        <f>primary!P62</f>
+        <f>primary!P63</f>
         <v>http://bioimages.vanderbilt.edu/vanderbilt/1-187</v>
       </c>
     </row>
     <row r="57" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="str">
-        <f>primary!A63</f>
+        <f>primary!A64</f>
         <v>1-454</v>
       </c>
       <c r="B57" s="1" t="str">
-        <f>primary!B63</f>
+        <f>primary!B64</f>
         <v>Magnolia grandiflora</v>
       </c>
       <c r="C57" s="1">
-        <f>primary!C63</f>
+        <f>primary!C64</f>
         <v>36.142907000000001</v>
       </c>
       <c r="D57" s="1">
-        <f>primary!D63</f>
+        <f>primary!D64</f>
         <v>-86.798353000000006</v>
       </c>
       <c r="E57" s="1" t="str">
-        <f>primary!E63</f>
+        <f>primary!E64</f>
         <v>62.5</v>
       </c>
       <c r="F57" s="14">
-        <f>primary!H63</f>
+        <f>primary!H64</f>
         <v>16.2</v>
       </c>
       <c r="G57" s="1">
-        <f>primary!K63</f>
+        <f>primary!K64</f>
         <v>14.75</v>
       </c>
       <c r="H57" s="22">
-        <f>primary!N63</f>
+        <f>primary!N64</f>
         <v>142.55379104330709</v>
       </c>
       <c r="I57" s="1" t="str">
-        <f>primary!O63</f>
+        <f>primary!O64</f>
         <v>northeastern magnolia in Magnolia Lawn along Magnolia Circle; another stem is 42.5 cm DBH</v>
       </c>
       <c r="J57" s="1" t="str">
-        <f>primary!P63</f>
+        <f>primary!P64</f>
         <v>http://bioimages.vanderbilt.edu/vanderbilt/12-193</v>
       </c>
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="str">
-        <f>primary!A64</f>
+        <f>primary!A65</f>
         <v>2-1027</v>
       </c>
       <c r="B58" s="1" t="str">
-        <f>primary!B64</f>
+        <f>primary!B65</f>
         <v>Magnolia grandiflora</v>
       </c>
       <c r="C58" s="1">
-        <f>primary!C64</f>
+        <f>primary!C65</f>
         <v>36.148297999999997</v>
       </c>
       <c r="D58" s="1">
-        <f>primary!D64</f>
+        <f>primary!D65</f>
         <v>-86.802287000000007</v>
       </c>
       <c r="E58" s="1">
-        <f>primary!E64</f>
+        <f>primary!E65</f>
         <v>61</v>
       </c>
       <c r="F58" s="14">
-        <f>primary!H64</f>
+        <f>primary!H65</f>
         <v>12.5</v>
       </c>
       <c r="G58" s="1">
-        <f>primary!K64</f>
+        <f>primary!K65</f>
         <v>14.5</v>
       </c>
       <c r="H58" s="22">
-        <f>primary!N64</f>
+        <f>primary!N65</f>
         <v>128.35375885826772</v>
       </c>
       <c r="I58" s="1" t="str">
-        <f>primary!O64</f>
+        <f>primary!O65</f>
         <v>east of Kirkland Hall; southwest of Kissam Quad; first tree north of curve in drive</v>
       </c>
       <c r="J58" s="1" t="str">
-        <f>primary!P64</f>
+        <f>primary!P65</f>
         <v>none</v>
       </c>
     </row>
     <row r="59" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="str">
-        <f>primary!A65</f>
+        <f>primary!A66</f>
         <v>1-375</v>
       </c>
       <c r="B59" s="1" t="str">
-        <f>primary!B65</f>
+        <f>primary!B66</f>
         <v>Cornus florida</v>
       </c>
       <c r="C59" s="1">
-        <f>primary!C65</f>
+        <f>primary!C66</f>
         <v>36.143264000000002</v>
       </c>
       <c r="D59" s="1">
-        <f>primary!D65</f>
+        <f>primary!D66</f>
         <v>-86.798715000000001</v>
       </c>
       <c r="E59" s="1">
-        <f>primary!E65</f>
+        <f>primary!E66</f>
         <v>32</v>
       </c>
       <c r="F59" s="14">
-        <f>primary!H65</f>
+        <f>primary!H66</f>
         <v>6.6</v>
       </c>
       <c r="G59" s="1">
-        <f>primary!K65</f>
+        <f>primary!K66</f>
         <v>8.85</v>
       </c>
       <c r="H59" s="22">
-        <f>primary!N65</f>
+        <f>primary!N66</f>
         <v>68.492899114173227</v>
       </c>
       <c r="I59" s="1" t="str">
-        <f>primary!O65</f>
+        <f>primary!O66</f>
         <v>west side of Magnolia Lawn on north side of the sidewalk that crosses the lawn; other stems: 24 cm and 21 cm DBH</v>
       </c>
       <c r="J59" s="1" t="str">
-        <f>primary!P65</f>
+        <f>primary!P66</f>
         <v>http://bioimages.vanderbilt.edu/vanderbilt/12-176</v>
       </c>
     </row>
     <row r="60" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="str">
-        <f>primary!A66</f>
+        <f>primary!A37</f>
         <v>2-319</v>
       </c>
       <c r="B60" s="1" t="str">
-        <f>primary!B66</f>
+        <f>primary!B37</f>
         <v>Magnolia grandiflora</v>
       </c>
       <c r="C60" s="1">
-        <f>primary!C66</f>
+        <f>primary!C37</f>
         <v>36.146718</v>
       </c>
       <c r="D60" s="1">
-        <f>primary!D66</f>
+        <f>primary!D37</f>
         <v>-86.802537000000001</v>
       </c>
       <c r="E60" s="1" t="str">
-        <f>primary!E66</f>
+        <f>primary!E37</f>
         <v>118</v>
       </c>
       <c r="F60" s="14">
-        <f>primary!H66</f>
-        <v>0</v>
+        <f>primary!H37</f>
+        <v>20</v>
       </c>
       <c r="G60" s="1">
-        <f>primary!K66</f>
-        <v>0</v>
+        <f>primary!K37</f>
+        <v>16.5</v>
       </c>
       <c r="H60" s="22">
-        <f>primary!N66</f>
-        <v>0</v>
+        <f>primary!N37</f>
+        <v>225.10200688976377</v>
       </c>
       <c r="I60" s="1" t="str">
-        <f>primary!O66</f>
+        <f>primary!O37</f>
         <v>between Rand and Old Central; note: also has another 59 cm dbh stem</v>
       </c>
       <c r="J60" s="1" t="str">
-        <f>primary!P66</f>
+        <f>primary!P37</f>
         <v>http://bioimages.vanderbilt.edu/vanderbilt/7-309</v>
       </c>
     </row>
@@ -24007,43 +24011,43 @@
     </row>
     <row r="69" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="str">
-        <f>primary!A51</f>
+        <f>primary!A52</f>
         <v>3-140</v>
       </c>
       <c r="B69" s="1" t="str">
-        <f>primary!B51</f>
+        <f>primary!B52</f>
         <v>Quercus muhlenbergii</v>
       </c>
       <c r="C69" s="1">
-        <f>primary!C51</f>
+        <f>primary!C52</f>
         <v>36.146026999999997</v>
       </c>
       <c r="D69" s="1">
-        <f>primary!D51</f>
+        <f>primary!D52</f>
         <v>-86.802841999999998</v>
       </c>
       <c r="E69" s="1" t="str">
-        <f>primary!E51</f>
+        <f>primary!E52</f>
         <v>97</v>
       </c>
       <c r="F69" s="14">
-        <f>primary!H51</f>
+        <f>primary!H52</f>
         <v>13.5</v>
       </c>
       <c r="G69" s="1">
-        <f>primary!K51</f>
+        <f>primary!K52</f>
         <v>22.5</v>
       </c>
       <c r="H69" s="22">
-        <f>primary!N51</f>
+        <f>primary!N52</f>
         <v>182.72323129921259</v>
       </c>
       <c r="I69" s="1" t="str">
-        <f>primary!O51</f>
+        <f>primary!O52</f>
         <v>By Station B post office entrance</v>
       </c>
       <c r="J69" s="1" t="str">
-        <f>primary!P51</f>
+        <f>primary!P52</f>
         <v>http://bioimages.vanderbilt.edu/vanderbilt/7-282</v>
       </c>
     </row>
@@ -24637,43 +24641,43 @@
     </row>
     <row r="84" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="str">
-        <f>primary!A52</f>
+        <f>primary!A53</f>
         <v>2-907</v>
       </c>
       <c r="B84" s="1" t="str">
-        <f>primary!B52</f>
+        <f>primary!B53</f>
         <v>Magnolia grandiflora</v>
       </c>
       <c r="C84" s="1">
-        <f>primary!C52</f>
+        <f>primary!C53</f>
         <v>36.148625000000003</v>
       </c>
       <c r="D84" s="1">
-        <f>primary!D52</f>
+        <f>primary!D53</f>
         <v>-86.802114000000003</v>
       </c>
       <c r="E84" s="1">
-        <f>primary!E52</f>
+        <f>primary!E53</f>
         <v>89</v>
       </c>
       <c r="F84" s="14">
-        <f>primary!H52</f>
+        <f>primary!H53</f>
         <v>18</v>
       </c>
       <c r="G84" s="1">
-        <f>primary!K52</f>
+        <f>primary!K53</f>
         <v>15</v>
       </c>
       <c r="H84" s="22">
-        <f>primary!N52</f>
+        <f>primary!N53</f>
         <v>181.44108464566929</v>
       </c>
       <c r="I84" s="1" t="str">
-        <f>primary!O52</f>
+        <f>primary!O53</f>
         <v>east of Kirkland Hall; southwest of Kissam Quad; away from the drive and closer to the dorms</v>
       </c>
       <c r="J84" s="1" t="str">
-        <f>primary!P52</f>
+        <f>primary!P53</f>
         <v>none</v>
       </c>
     </row>

</xml_diff>

<commit_message>
updated database with Vandy/Barnard trees
</commit_message>
<xml_diff>
--- a/measured-trees.xlsx
+++ b/measured-trees.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\github\database\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="13290" windowHeight="14040" tabRatio="347"/>
   </bookViews>
@@ -13,7 +18,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">primary!$A$3:$P$104</definedName>
   </definedNames>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
@@ -24,7 +29,7 @@
     <author>Steven J Baskauf</author>
   </authors>
   <commentList>
-    <comment ref="I4" authorId="0">
+    <comment ref="I4" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -48,7 +53,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E11" authorId="1">
+    <comment ref="E11" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -72,7 +77,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H11" authorId="1">
+    <comment ref="H11" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -96,7 +101,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I17" authorId="0">
+    <comment ref="I17" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -120,7 +125,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H21" authorId="0">
+    <comment ref="H21" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -144,7 +149,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E22" authorId="0">
+    <comment ref="E22" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -168,7 +173,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H22" authorId="1">
+    <comment ref="H22" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -192,7 +197,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I22" authorId="0">
+    <comment ref="I22" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -216,7 +221,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K22" authorId="0">
+    <comment ref="K22" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -240,7 +245,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A23" authorId="0">
+    <comment ref="A23" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -264,7 +269,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I25" authorId="0">
+    <comment ref="I25" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -288,7 +293,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I27" authorId="0">
+    <comment ref="I27" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -312,7 +317,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E34" authorId="1">
+    <comment ref="E34" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -336,7 +341,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H34" authorId="1">
+    <comment ref="H34" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -360,7 +365,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I38" authorId="0">
+    <comment ref="I38" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -384,7 +389,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H39" authorId="1">
+    <comment ref="H39" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -408,7 +413,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K39" authorId="1">
+    <comment ref="K39" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -432,7 +437,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I40" authorId="0">
+    <comment ref="I40" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -456,7 +461,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I42" authorId="0">
+    <comment ref="I42" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -480,7 +485,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E44" authorId="1">
+    <comment ref="E44" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -504,7 +509,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H44" authorId="1">
+    <comment ref="H44" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -528,7 +533,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B45" authorId="1">
+    <comment ref="B45" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -552,7 +557,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H47" authorId="1">
+    <comment ref="H47" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -576,7 +581,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I47" authorId="0">
+    <comment ref="I47" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -600,7 +605,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K47" authorId="0">
+    <comment ref="K47" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -624,7 +629,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E49" authorId="1">
+    <comment ref="E49" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -648,7 +653,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H49" authorId="1">
+    <comment ref="H49" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -672,7 +677,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H52" authorId="0">
+    <comment ref="H52" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -696,7 +701,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H57" authorId="0">
+    <comment ref="H57" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -720,7 +725,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E58" authorId="0">
+    <comment ref="E58" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -744,7 +749,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="N58" authorId="1">
+    <comment ref="N58" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -768,7 +773,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E59" authorId="1">
+    <comment ref="E59" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -792,7 +797,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H60" authorId="0">
+    <comment ref="H60" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -816,7 +821,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E61" authorId="1">
+    <comment ref="E61" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -840,7 +845,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H61" authorId="1">
+    <comment ref="H61" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -864,7 +869,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E63" authorId="1">
+    <comment ref="E63" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -888,7 +893,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H63" authorId="1">
+    <comment ref="H63" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -912,7 +917,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K63" authorId="1">
+    <comment ref="K63" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -936,7 +941,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="N63" authorId="1">
+    <comment ref="N63" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -960,7 +965,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A72" authorId="0">
+    <comment ref="A72" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -984,7 +989,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A82" authorId="0">
+    <comment ref="A82" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1008,7 +1013,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E105" authorId="1">
+    <comment ref="E105" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1032,7 +1037,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B107" authorId="0">
+    <comment ref="B107" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1056,7 +1061,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E108" authorId="0">
+    <comment ref="E108" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1080,12 +1085,40 @@
         </r>
       </text>
     </comment>
+    <comment ref="E110" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>additional trunks: 63 cm and 45 cm</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E113" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Additional trunks: 60 cm and 32 cm</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="785" uniqueCount="427">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="825" uniqueCount="447">
   <si>
     <t>ID</t>
   </si>
@@ -2366,6 +2399,66 @@
   </si>
   <si>
     <t>east of Kirkland Hall; southwest of Kissam Quad; first tree north of curve in drive</t>
+  </si>
+  <si>
+    <t>2-468</t>
+  </si>
+  <si>
+    <t>2016-05-11</t>
+  </si>
+  <si>
+    <t>west of Vanderbilt Hall, to be removed for construction</t>
+  </si>
+  <si>
+    <t>36.148395</t>
+  </si>
+  <si>
+    <t>-86.804136</t>
+  </si>
+  <si>
+    <t>2-910</t>
+  </si>
+  <si>
+    <t>36.1488</t>
+  </si>
+  <si>
+    <t>-86.803725</t>
+  </si>
+  <si>
+    <t>north of Barnhard Hall, to be removed for construction</t>
+  </si>
+  <si>
+    <t>2-616</t>
+  </si>
+  <si>
+    <t>36.148811</t>
+  </si>
+  <si>
+    <t>-86.80329</t>
+  </si>
+  <si>
+    <t>northeast of Barnhard Hall, to be removed for construction</t>
+  </si>
+  <si>
+    <t>2-596</t>
+  </si>
+  <si>
+    <t>36.148651</t>
+  </si>
+  <si>
+    <t>-86.803173</t>
+  </si>
+  <si>
+    <t>2-891</t>
+  </si>
+  <si>
+    <t>36.148385</t>
+  </si>
+  <si>
+    <t>-86.803485</t>
+  </si>
+  <si>
+    <t>south of Barnhard Hall, to be removed for construction</t>
   </si>
 </sst>
 </file>
@@ -2956,7 +3049,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2967,11 +3060,11 @@
   <dimension ref="A1:Q684"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <pane xSplit="3330" ySplit="600" topLeftCell="G32" activePane="bottomLeft"/>
+      <pane xSplit="3330" ySplit="600" topLeftCell="A76" activePane="bottomRight"/>
       <selection activeCell="A22" sqref="A22"/>
       <selection pane="topRight" activeCell="K3" sqref="K3"/>
-      <selection pane="bottomLeft" activeCell="A37" sqref="A37:XFD37"/>
-      <selection pane="bottomRight" activeCell="H68" sqref="H68"/>
+      <selection pane="bottomLeft" activeCell="B111" sqref="B111"/>
+      <selection pane="bottomRight" activeCell="O115" sqref="O115"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8476,116 +8569,261 @@
       </c>
     </row>
     <row r="110" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="E110" s="26"/>
+      <c r="A110" s="1" t="s">
+        <v>427</v>
+      </c>
+      <c r="B110" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="C110" s="1" t="s">
+        <v>430</v>
+      </c>
+      <c r="D110" s="1" t="s">
+        <v>431</v>
+      </c>
+      <c r="E110" s="26">
+        <v>63</v>
+      </c>
       <c r="F110" s="26">
         <f t="shared" ref="F110:F129" si="16">E110/2.54</f>
-        <v>0</v>
-      </c>
-      <c r="H110" s="14"/>
+        <v>24.803149606299211</v>
+      </c>
+      <c r="G110" s="24" t="s">
+        <v>428</v>
+      </c>
+      <c r="H110" s="14">
+        <v>19.600000000000001</v>
+      </c>
       <c r="I110" s="21">
         <f t="shared" ref="I110:I130" si="17">H110*3.281</f>
-        <v>0</v>
-      </c>
-      <c r="J110" s="7"/>
-      <c r="K110" s="29"/>
+        <v>64.307600000000008</v>
+      </c>
+      <c r="J110" s="7" t="s">
+        <v>428</v>
+      </c>
+      <c r="K110" s="29">
+        <v>15.5</v>
+      </c>
       <c r="L110" s="30">
         <f t="shared" ref="L110:L130" si="18">K110*3.281</f>
-        <v>0</v>
+        <v>50.855499999999999</v>
+      </c>
+      <c r="M110" s="27" t="s">
+        <v>428</v>
       </c>
       <c r="N110" s="15">
         <f t="shared" ref="N110:N130" si="19">IF(K110=0,0,E110/2.54*3.14159+H110*3.281+K110*3.281/4)</f>
-        <v>0</v>
+        <v>154.94280177165356</v>
+      </c>
+      <c r="O110" s="1" t="s">
+        <v>429</v>
       </c>
     </row>
     <row r="111" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="E111" s="26"/>
+      <c r="A111" s="1" t="s">
+        <v>432</v>
+      </c>
+      <c r="B111" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C111" s="1" t="s">
+        <v>433</v>
+      </c>
+      <c r="D111" s="1" t="s">
+        <v>434</v>
+      </c>
+      <c r="E111" s="26">
+        <v>115</v>
+      </c>
       <c r="F111" s="26">
         <f t="shared" si="16"/>
-        <v>0</v>
-      </c>
-      <c r="H111" s="14"/>
+        <v>45.275590551181104</v>
+      </c>
+      <c r="G111" s="145" t="s">
+        <v>428</v>
+      </c>
+      <c r="H111" s="14">
+        <v>16</v>
+      </c>
       <c r="I111" s="21">
         <f t="shared" si="17"/>
-        <v>0</v>
-      </c>
-      <c r="J111" s="7"/>
-      <c r="K111" s="29"/>
+        <v>52.496000000000002</v>
+      </c>
+      <c r="J111" s="134" t="s">
+        <v>428</v>
+      </c>
+      <c r="K111" s="29">
+        <v>18</v>
+      </c>
       <c r="L111" s="30">
         <f t="shared" si="18"/>
-        <v>0</v>
+        <v>59.058</v>
+      </c>
+      <c r="M111" s="147" t="s">
+        <v>428</v>
       </c>
       <c r="N111" s="15">
         <f t="shared" si="19"/>
-        <v>0</v>
+        <v>209.49784251968504</v>
+      </c>
+      <c r="O111" s="1" t="s">
+        <v>435</v>
       </c>
     </row>
     <row r="112" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="E112" s="26"/>
+      <c r="A112" s="1" t="s">
+        <v>436</v>
+      </c>
+      <c r="B112" s="130" t="s">
+        <v>55</v>
+      </c>
+      <c r="C112" s="1" t="s">
+        <v>437</v>
+      </c>
+      <c r="D112" s="1" t="s">
+        <v>438</v>
+      </c>
+      <c r="E112" s="26">
+        <v>76</v>
+      </c>
       <c r="F112" s="26">
         <f t="shared" si="16"/>
-        <v>0</v>
-      </c>
-      <c r="H112" s="14"/>
+        <v>29.921259842519685</v>
+      </c>
+      <c r="G112" s="145" t="s">
+        <v>428</v>
+      </c>
+      <c r="H112" s="14">
+        <v>13.7</v>
+      </c>
       <c r="I112" s="21">
         <f t="shared" si="17"/>
-        <v>0</v>
-      </c>
-      <c r="J112" s="7"/>
-      <c r="K112" s="29"/>
+        <v>44.9497</v>
+      </c>
+      <c r="J112" s="134" t="s">
+        <v>428</v>
+      </c>
+      <c r="K112" s="29">
+        <v>11</v>
+      </c>
       <c r="L112" s="30">
         <f t="shared" si="18"/>
-        <v>0</v>
+        <v>36.091000000000001</v>
+      </c>
+      <c r="M112" s="147" t="s">
+        <v>428</v>
       </c>
       <c r="N112" s="15">
         <f t="shared" si="19"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="113" spans="5:14" x14ac:dyDescent="0.25">
-      <c r="E113" s="26"/>
+        <v>147.97278070866142</v>
+      </c>
+      <c r="O112" s="130" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="113" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A113" s="1" t="s">
+        <v>440</v>
+      </c>
+      <c r="B113" s="130" t="s">
+        <v>55</v>
+      </c>
+      <c r="C113" s="1" t="s">
+        <v>441</v>
+      </c>
+      <c r="D113" s="1" t="s">
+        <v>442</v>
+      </c>
+      <c r="E113" s="26">
+        <v>74</v>
+      </c>
       <c r="F113" s="26">
         <f t="shared" si="16"/>
-        <v>0</v>
-      </c>
-      <c r="H113" s="14"/>
+        <v>29.133858267716533</v>
+      </c>
+      <c r="G113" s="145" t="s">
+        <v>428</v>
+      </c>
+      <c r="H113" s="14">
+        <v>14</v>
+      </c>
       <c r="I113" s="21">
         <f t="shared" si="17"/>
-        <v>0</v>
-      </c>
-      <c r="J113" s="7"/>
-      <c r="K113" s="29"/>
+        <v>45.934000000000005</v>
+      </c>
+      <c r="J113" s="134" t="s">
+        <v>428</v>
+      </c>
+      <c r="K113" s="29">
+        <v>15.5</v>
+      </c>
       <c r="L113" s="30">
         <f t="shared" si="18"/>
-        <v>0</v>
+        <v>50.855499999999999</v>
+      </c>
+      <c r="M113" s="147" t="s">
+        <v>428</v>
       </c>
       <c r="N113" s="15">
         <f t="shared" si="19"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="114" spans="5:14" x14ac:dyDescent="0.25">
-      <c r="E114" s="26"/>
+        <v>150.17451279527558</v>
+      </c>
+      <c r="O113" s="130" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="114" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A114" s="1" t="s">
+        <v>443</v>
+      </c>
+      <c r="B114" s="130" t="s">
+        <v>55</v>
+      </c>
+      <c r="C114" s="1" t="s">
+        <v>444</v>
+      </c>
+      <c r="D114" s="1" t="s">
+        <v>445</v>
+      </c>
+      <c r="E114" s="26">
+        <v>101</v>
+      </c>
       <c r="F114" s="26">
         <f t="shared" si="16"/>
-        <v>0</v>
-      </c>
-      <c r="H114" s="14"/>
+        <v>39.763779527559052</v>
+      </c>
+      <c r="G114" s="145" t="s">
+        <v>428</v>
+      </c>
+      <c r="H114" s="14">
+        <v>15</v>
+      </c>
       <c r="I114" s="21">
         <f t="shared" si="17"/>
-        <v>0</v>
-      </c>
-      <c r="J114" s="7"/>
-      <c r="K114" s="29"/>
+        <v>49.215000000000003</v>
+      </c>
+      <c r="J114" s="134" t="s">
+        <v>428</v>
+      </c>
+      <c r="K114" s="29">
+        <v>14.25</v>
+      </c>
       <c r="L114" s="30">
         <f t="shared" si="18"/>
-        <v>0</v>
+        <v>46.754249999999999</v>
+      </c>
+      <c r="M114" s="147" t="s">
+        <v>428</v>
       </c>
       <c r="N114" s="15">
         <f t="shared" si="19"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="115" spans="5:14" x14ac:dyDescent="0.25">
+        <v>185.82505462598425</v>
+      </c>
+      <c r="O114" s="130" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="115" spans="1:15" x14ac:dyDescent="0.25">
       <c r="E115" s="26"/>
       <c r="F115" s="26">
         <f t="shared" si="16"/>
@@ -8607,7 +8845,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="116" spans="5:14" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:15" x14ac:dyDescent="0.25">
       <c r="E116" s="26"/>
       <c r="F116" s="26">
         <f t="shared" si="16"/>
@@ -8629,7 +8867,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="117" spans="5:14" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:15" x14ac:dyDescent="0.25">
       <c r="E117" s="26"/>
       <c r="F117" s="26">
         <f t="shared" si="16"/>
@@ -8651,7 +8889,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="118" spans="5:14" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:15" x14ac:dyDescent="0.25">
       <c r="E118" s="26"/>
       <c r="F118" s="26">
         <f t="shared" si="16"/>
@@ -8673,7 +8911,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="119" spans="5:14" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:15" x14ac:dyDescent="0.25">
       <c r="E119" s="26"/>
       <c r="F119" s="26">
         <f t="shared" si="16"/>
@@ -8695,7 +8933,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="120" spans="5:14" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:15" x14ac:dyDescent="0.25">
       <c r="E120" s="26"/>
       <c r="F120" s="26">
         <f t="shared" si="16"/>
@@ -8717,7 +8955,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="121" spans="5:14" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:15" x14ac:dyDescent="0.25">
       <c r="E121" s="26"/>
       <c r="F121" s="26">
         <f t="shared" si="16"/>
@@ -8739,7 +8977,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="122" spans="5:14" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:15" x14ac:dyDescent="0.25">
       <c r="E122" s="26"/>
       <c r="F122" s="26">
         <f t="shared" si="16"/>
@@ -8761,7 +8999,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="123" spans="5:14" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:15" x14ac:dyDescent="0.25">
       <c r="E123" s="26"/>
       <c r="F123" s="26">
         <f t="shared" si="16"/>
@@ -8783,7 +9021,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="124" spans="5:14" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:15" x14ac:dyDescent="0.25">
       <c r="E124" s="26"/>
       <c r="F124" s="26">
         <f t="shared" si="16"/>
@@ -8805,7 +9043,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="125" spans="5:14" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:15" x14ac:dyDescent="0.25">
       <c r="E125" s="26"/>
       <c r="F125" s="26">
         <f t="shared" si="16"/>
@@ -8827,7 +9065,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="126" spans="5:14" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:15" x14ac:dyDescent="0.25">
       <c r="E126" s="26"/>
       <c r="F126" s="26">
         <f t="shared" si="16"/>
@@ -8849,7 +9087,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="127" spans="5:14" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:15" x14ac:dyDescent="0.25">
       <c r="E127" s="26"/>
       <c r="F127" s="26">
         <f t="shared" si="16"/>
@@ -8871,7 +9109,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="128" spans="5:14" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:15" x14ac:dyDescent="0.25">
       <c r="E128" s="26"/>
       <c r="F128" s="26">
         <f t="shared" si="16"/>

</xml_diff>

<commit_message>
updated URLs for Vandy/Barnard trees
</commit_message>
<xml_diff>
--- a/measured-trees.xlsx
+++ b/measured-trees.xlsx
@@ -37,7 +37,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Steve Baskauf:</t>
         </r>
@@ -46,7 +46,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 measured in feet by surveying class 2014-04</t>
@@ -61,7 +61,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Steven J Baskauf:</t>
         </r>
@@ -70,7 +70,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 measured by SSMV students</t>
@@ -85,7 +85,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Steven J Baskauf:</t>
         </r>
@@ -94,7 +94,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 measured by SSMV students.  Verify this.</t>
@@ -109,7 +109,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Steve Baskauf:</t>
         </r>
@@ -118,7 +118,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 measured in feet by surveying class 2014-04</t>
@@ -133,7 +133,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Steve Baskauf:</t>
         </r>
@@ -142,7 +142,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 measured by Vanderbilt School for Science and Math Students</t>
@@ -181,7 +181,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Steve Baskauf:</t>
         </r>
@@ -190,7 +190,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 measured in feet by Vanderbilt School for Science and Math Students</t>
@@ -205,7 +205,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Steve Baskauf:</t>
         </r>
@@ -214,7 +214,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 measured in feet by Vanderbilt School for Science and Math Students</t>
@@ -229,7 +229,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Steven J Baskauf:</t>
         </r>
@@ -238,7 +238,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 measured by SSMV students</t>
@@ -253,7 +253,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Steven J Baskauf:</t>
         </r>
@@ -262,7 +262,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 measured by SSMV students, verify this</t>
@@ -277,7 +277,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Steve Baskauf:</t>
         </r>
@@ -286,7 +286,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 measured in feet by Vanderbilt School for Science and Math Students</t>
@@ -301,7 +301,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Steven J Baskauf:</t>
         </r>
@@ -310,7 +310,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 measured by SSMV students</t>
@@ -325,7 +325,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Steven J Baskauf:</t>
         </r>
@@ -334,7 +334,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 measured by SSMV students</t>
@@ -349,7 +349,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Steve Baskauf:</t>
         </r>
@@ -358,7 +358,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 measured in feet by surveying class</t>
@@ -373,7 +373,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Steve Baskauf:</t>
         </r>
@@ -382,7 +382,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 measured in feet by Vanderbilt School for Science and Math Students</t>
@@ -397,7 +397,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Steven J Baskauf:</t>
         </r>
@@ -406,7 +406,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 measured by SSMV students as 107.5 cm on 2014-08-20.  Note: splits at head height to two trunks</t>
@@ -421,7 +421,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Steven J Baskauf:</t>
         </r>
@@ -430,7 +430,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 measured by SSMV students at 20.4 m on 2014-08-20</t>
@@ -445,7 +445,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>cut down in 2014</t>
         </r>
@@ -459,7 +459,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Steven J Baskauf:</t>
         </r>
@@ -468,7 +468,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 large branch about 90 years old, so tree is about 100 ya in 2014</t>
@@ -483,7 +483,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Steven J Baskauf:</t>
         </r>
@@ -492,7 +492,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 measured by SSMV students</t>
@@ -507,7 +507,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Steve Baskauf:</t>
         </r>
@@ -516,7 +516,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 measured by vssm students</t>
@@ -531,7 +531,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Steve Baskauf:</t>
         </r>
@@ -540,7 +540,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 measured by vssm</t>
@@ -555,7 +555,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Steven J Baskauf:</t>
         </r>
@@ -564,7 +564,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 measured by SSMV students</t>
@@ -579,7 +579,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Steven J Baskauf:</t>
         </r>
@@ -588,7 +588,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 measured by SSMV students</t>
@@ -603,7 +603,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Steve Baskauf:</t>
         </r>
@@ -612,7 +612,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 measured by Vanderbilt School for Science and Math Students</t>
@@ -627,7 +627,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Steve Baskauf:</t>
         </r>
@@ -636,7 +636,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 measured by Vanderbilt School for Science and Math Students</t>
@@ -675,7 +675,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Steven J Baskauf:</t>
         </r>
@@ -684,7 +684,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 would be 218 if a single stem</t>
@@ -699,7 +699,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Steven J Baskauf:</t>
         </r>
@@ -708,7 +708,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 Note: this tree is larger than its diameter would indicate because a number of branches that were touching the ground have sprouted and are now auxillary trees around the main one (clones)</t>
@@ -723,7 +723,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Steve Baskauf:</t>
         </r>
@@ -732,7 +732,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 measured by Vanderbilt School for Science and Math Students</t>
@@ -747,7 +747,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Steven J Baskauf:</t>
         </r>
@@ -756,7 +756,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 measured by SSMV students</t>
@@ -771,7 +771,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Steven J Baskauf:</t>
         </r>
@@ -780,7 +780,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 measured by SSMV students</t>
@@ -795,7 +795,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Steven J Baskauf:</t>
         </r>
@@ -804,7 +804,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 measured by SSMV students to be 127 cm dbh on 2014-08-20.  However, I checked it and it actually has a three-way split trunk that forks below breast height, with 58, 56, and 52 cm trunks.</t>
@@ -819,7 +819,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Steven J Baskauf:</t>
         </r>
@@ -828,7 +828,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 measured by SSMV students to be 22.5 m on 2014-08-20</t>
@@ -843,7 +843,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Steven J Baskauf:</t>
         </r>
@@ -852,7 +852,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 measured at 13.9 m on 2014-08-20 by SSMV students</t>
@@ -867,7 +867,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Steven J Baskauf:</t>
         </r>
@@ -876,7 +876,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 Note: this value underestimates the tree's size.  It would probably be well over 200 points if the trunk didn't split into three</t>
@@ -891,7 +891,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Steve Baskauf:</t>
         </r>
@@ -900,7 +900,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 cut down in 2015</t>
@@ -1011,7 +1011,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>additional trunks: 63 cm and 45 cm</t>
         </r>
@@ -1025,7 +1025,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Additional trunks: 60 cm and 32 cm</t>
         </r>
@@ -1039,7 +1039,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Steve Baskauf:</t>
         </r>
@@ -1048,7 +1048,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 This record is really messed up.  The ID number is incorrect for the location description and the description of the tree as having three trunks is also wrong relative to the actual tree at that location.  I have corrected the tree at this location with data from 2016 but I don't know what tree was actually being described here.</t>
@@ -1087,7 +1087,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Steven J Baskauf:</t>
         </r>
@@ -1096,7 +1096,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 measured by SSMV students, my previous estimate was 28 m, so verification would be good</t>
@@ -1111,7 +1111,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Steve Baskauf:</t>
         </r>
@@ -1120,7 +1120,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 measured by vssm students</t>
@@ -1135,7 +1135,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Steve Baskauf:</t>
         </r>
@@ -1144,7 +1144,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 measured by vssm students</t>
@@ -1156,7 +1156,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="833" uniqueCount="453">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="838" uniqueCount="458">
   <si>
     <t>ID</t>
   </si>
@@ -2515,6 +2515,21 @@
   </si>
   <si>
     <t>http://bioimages.vanderbilt.edu/vanderbilt/2-83</t>
+  </si>
+  <si>
+    <t>http://bioimages.vanderbilt.edu/vanderbilt/2-152</t>
+  </si>
+  <si>
+    <t>http://bioimages.vanderbilt.edu/vanderbilt/2-158</t>
+  </si>
+  <si>
+    <t>http://bioimages.vanderbilt.edu/vanderbilt/2-94</t>
+  </si>
+  <si>
+    <t>http://bioimages.vanderbilt.edu/vanderbilt/2-99</t>
+  </si>
+  <si>
+    <t>http://bioimages.vanderbilt.edu/vanderbilt/2-116</t>
   </si>
 </sst>
 </file>
@@ -2525,7 +2540,7 @@
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="0.000000"/>
   </numFmts>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2563,21 +2578,9 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
-    </font>
-    <font>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
@@ -2673,10 +2676,10 @@
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="175">
+  <cellXfs count="176">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -2839,7 +2842,7 @@
     <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
@@ -2848,10 +2851,11 @@
     <xf numFmtId="49" fontId="0" fillId="7" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" xfId="2" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" xfId="2" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="1" fontId="0" fillId="7" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
@@ -3137,11 +3141,11 @@
   <dimension ref="A1:Q683"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <pane xSplit="3330" ySplit="600" topLeftCell="A4" activePane="bottomRight"/>
+      <pane xSplit="3330" ySplit="600" topLeftCell="C4" activePane="bottomRight"/>
       <selection activeCell="A22" sqref="A22"/>
       <selection pane="topRight" activeCell="C22" sqref="C22:D22"/>
-      <selection pane="bottomLeft" activeCell="A72" sqref="A72:XFD72"/>
-      <selection pane="bottomRight" activeCell="A46" sqref="A46"/>
+      <selection pane="bottomLeft" activeCell="A49" sqref="A49:XFD49"/>
+      <selection pane="bottomRight" activeCell="P115" sqref="P115"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8696,6 +8700,9 @@
       <c r="O110" s="1" t="s">
         <v>429</v>
       </c>
+      <c r="P110" s="130" t="s">
+        <v>453</v>
+      </c>
     </row>
     <row r="111" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A111" s="1" t="s">
@@ -8747,6 +8754,9 @@
       <c r="O111" s="1" t="s">
         <v>435</v>
       </c>
+      <c r="P111" s="130" t="s">
+        <v>454</v>
+      </c>
     </row>
     <row r="112" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A112" s="1" t="s">
@@ -8798,6 +8808,9 @@
       <c r="O112" s="130" t="s">
         <v>439</v>
       </c>
+      <c r="P112" s="175" t="s">
+        <v>455</v>
+      </c>
     </row>
     <row r="113" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A113" s="1" t="s">
@@ -8849,6 +8862,9 @@
       <c r="O113" s="130" t="s">
         <v>439</v>
       </c>
+      <c r="P113" s="130" t="s">
+        <v>456</v>
+      </c>
     </row>
     <row r="114" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A114" s="1" t="s">
@@ -8899,6 +8915,9 @@
       </c>
       <c r="O114" s="130" t="s">
         <v>446</v>
+      </c>
+      <c r="P114" s="129" t="s">
+        <v>457</v>
       </c>
     </row>
     <row r="115" spans="1:17" x14ac:dyDescent="0.25">

</xml_diff>